<commit_message>
sua file robot json
</commit_message>
<xml_diff>
--- a/DataJson/tien_nhan_vat/robot_json.xlsx
+++ b/DataJson/tien_nhan_vat/robot_json.xlsx
@@ -5,10 +5,10 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\trinh\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\FrontEndProject\DataJson\tien_nhan_vat\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D90DAA9-C54C-4BF1-AF2C-00B385741497}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51464191-B188-41BA-AC22-F4511CC94C9E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="264" uniqueCount="205">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="266" uniqueCount="207">
   <si>
     <t>name</t>
   </si>
@@ -75,13 +75,6 @@
     <t>YW720315</t>
   </si>
   <si>
-    <t>&lt;p&gt;Super Wings là bộ phim hoạt hình nổi tiếng đến từ Hàn Quốc, nhận được nhiều sự yêu thích của trẻ em trên toàn thế giới.&lt;/p&gt;
-&lt;p&gt;Robot biến hình kết hợp xe cứu hộ nhỏ - cảnh sát Paul&lt;/p&gt;
-&lt;p&gt;- Biến đổi dễ dàng từ robot cao gần 7 inch thành xe cứu hộ nhỏ qua 3 bước biến hình đơn giản.&lt;br&gt; - Với bánh xe cao su và thang cứu hộ mở rộng tạo cảm giác chân thật khi chơi.&lt;br&gt; - Kích thích tư duy thông qua trò chơi, rèn luyện ngón tay và trí tưởng tượng của bé khi hoá thân vào nhân vật yêu thích.&lt;/p&gt;
-&lt;p&gt;Thông tin sản phẩm:&lt;br&gt; - Sản phẩm sử dụng nhựa cao cấp đảm bảo an toàn cho bé. &lt;br&gt; - Thích hợp cho bé từ 3 tuổi trở lên.&lt;br&gt; - Sản phẩm không sử dụng Pin&lt;/p&gt;
-&lt;p&gt;&lt;img style="vertical-align: baseline; display: block; margin-left: auto; margin-right: auto;" src="https://www.mykingdom.com.vn/media/wysiwyg/Long/Line_Robot_bi_n_h_nh_si_u_xe_c_u_h_nh_.png" width="711" height="400"&gt;&lt;/p&gt;</t>
-  </si>
-  <si>
     <t>https://www.mykingdom.com.vn/media/catalog/product/cache/a237138a07ed0dd2cc8a6fa440635ea6/magento/SUPERWINGS/YW720315/YW720315_1.jpg</t>
   </si>
   <si>
@@ -100,26 +93,6 @@
     <t>YW720314</t>
   </si>
   <si>
-    <t>&lt;h2&gt;&lt;span style="font-size: 12px;"&gt;&lt;/span&gt;&lt;/h2&gt;
-&lt;h2&gt;Robot biến hình kết hợp xe cứu hộ nhỏ - Dizzy Lốc Xoáy&lt;/h2&gt;
-&lt;h2&gt;&lt;span style="font-size: 12px;"&gt;Super Wings là bộ phim hoạt hình nổi tiếng đến từ Hàn Quốc, nhận được nhiều sự yêu thích của trẻ em trên toàn thế giới.&lt;/span&gt;&lt;/h2&gt;
-&lt;p&gt;Robot biến hình kết hợp xe cứu hộ nhỏ - Dizzy Lốc Xoáy&lt;/p&gt;
-&lt;p&gt;- Biến đổi dễ dàng từ robot cao gần 7 inch thành xe cứu hộ nhỏ qua 3 bước biến hình đơn giản.&lt;br&gt; - Với bánh xe cao su và thang cứu hộ mở rộng tạo cảm giác chân thật khi chơi.&lt;br&gt; - Kích thích tư duy thông qua trò chơi, rèn luyện ngón tay và trí tưởng tượng của bé khi hoá thân vào nhân vật yêu thích.&lt;/p&gt;
-&lt;h3&gt;Thông tin sản phẩm:&lt;/h3&gt;
-&lt;p&gt;- Sản phẩm sử dụng nhựa cao cấp đảm bảo an toàn cho bé. &lt;br&gt; - Thích hợp cho bé từ 3 tuổi trở lên.&lt;br&gt; - Sản phẩm không sử dụng Pin&lt;/p&gt;
-&lt;p&gt;&lt;img style="vertical-align: baseline; display: block; margin-left: auto; margin-right: auto;" src="https://www.mykingdom.com.vn/media/wysiwyg/Long/Line_Robot_bi_n_h_nh_si_u_xe_c_u_h_nh_.png" width="711" height="400"&gt;&lt;/p&gt;
-&lt;p&gt;&lt;br&gt; - Sản phẩm không sử dụng Pin&lt;/p&gt;
-&lt;table class="MsoNormalTable" style="width: 623px; border-collapse: collapse;" border="0" cellspacing="0" cellpadding="0"&gt;
-&lt;tbody&gt;
-&lt;tr style="mso-yfti-irow: 0; mso-yfti-firstrow: yes; mso-yfti-lastrow: yes; height: 14.25pt;"&gt;
-&lt;td style="width: 364.45pt; border: solid windowtext 1.0pt; border-top: none; mso-border-left-alt: solid windowtext .5pt; mso-border-bottom-alt: solid windowtext .5pt; mso-border-right-alt: solid windowtext .5pt; padding: 0in 5.4pt 0in 5.4pt; height: 14.25pt;" nowrap="nowrap" width="486"&gt;
-&lt;p class="MsoNormal" style="margin-bottom: .0001pt; text-align: justify; line-height: normal;"&gt;&lt;span style="font-size: 10.0pt; font-family: 'Tahoma','sans-serif'; mso-fareast-font-family: 'Times New Roman'; color: black;"&gt;Robot biến hình kết hợp xe cứu hộ nhỏ&lt;span style="mso-spacerun: yes;"&gt;&amp;nbsp; &lt;/span&gt;- Dizzy Lốc Xoáy&lt;/span&gt;&lt;/p&gt;
-&lt;/td&gt;
-&lt;/tr&gt;
-&lt;/tbody&gt;
-&lt;/table&gt;</t>
-  </si>
-  <si>
     <t>https://www.mykingdom.com.vn/media/catalog/product/cache/a237138a07ed0dd2cc8a6fa440635ea6/magento/SUPERWINGS/YW720314/YW720314_1.jpg</t>
   </si>
   <si>
@@ -138,16 +111,6 @@
     <t>YW720312</t>
   </si>
   <si>
-    <t>&lt;h2&gt;Robot biến hình kết hợp xe cứu hộ nhỏ - Donnie Thông Minh&lt;/h2&gt;
-&lt;p&gt;Super Wings là bộ phim hoạt hình nổi tiếng đến từ Hàn Quốc, nhận được nhiều sự yêu thích của trẻ em trên toàn thế giới.&lt;/p&gt;
-&lt;p&gt;&lt;/p&gt;
-&lt;p&gt;- Biến đổi dễ dàng từ robot cao gần 7 inch thành xe cứu hộ nhỏ qua 3 bước biến hình đơn giản.&lt;br&gt; - Với bánh xe cao su và thang cứu hộ mở rộng tạo cảm giác chân thật khi chơi.&lt;br&gt; - Kích thích tư duy thông qua trò chơi, rèn luyện ngón tay và trí tưởng tượng của bé khi hoá thân vào nhân vật yêu thích.&lt;/p&gt;
-&lt;h3&gt;Thông tin sản phẩm:&lt;/h3&gt;
-&lt;p&gt;- Sản phẩm sử dụng nhựa cao cấp đảm bảo an toàn cho bé. &lt;br&gt;- Thích hợp cho bé từ 3 tuổi trở lên.&lt;/p&gt;
-&lt;p&gt;&lt;img style="vertical-align: baseline; display: block; margin-left: auto; margin-right: auto;" src="https://www.mykingdom.com.vn/media/wysiwyg/Long/Line_Robot_bi_n_h_nh_si_u_xe_c_u_h_nh_.png" width="711" height="400"&gt;&lt;/p&gt;
-&lt;p&gt;&lt;br&gt; - Sản phẩm không sử dụng Pin&lt;/p&gt;</t>
-  </si>
-  <si>
     <t>https://www.mykingdom.com.vn/media/catalog/product/cache/a237138a07ed0dd2cc8a6fa440635ea6/magento/SUPERWINGS/YW720312/YW720312_1.jpg</t>
   </si>
   <si>
@@ -164,16 +127,6 @@
   </si>
   <si>
     <t>YW720311</t>
-  </si>
-  <si>
-    <t>&lt;h2&gt;ROBOT BIẾN HÌNH KÊT HỢP XE CỨU HỘ NHỎ JETT TIA CHỚP&lt;/h2&gt;
-&lt;p&gt;Super Wings là bộ phim hoạt hình nổi tiếng đến từ Hàn Quốc, nhận được nhiều sự yêu thích của trẻ em trên toàn thế giới.&lt;/p&gt;
-&lt;p&gt;Robot biến hình kết hợp xe cứu hộ nhỏ - Jett Tia Chớp&lt;/p&gt;
-&lt;p&gt;- Biến đổi dễ dàng từ robot cao gần 7 inch thành xe cứu hộ nhỏ qua 3 bước biến hình đơn giản.&lt;br&gt; - Với bánh xe cao su và thang cứu hộ mở rộng tạo cảm giác chân thật khi chơi.&lt;br&gt; - Kích thích tư duy thông qua trò chơi, rèn luyện ngón tay và trí tưởng tượng của bé khi hoá thân vào nhân vật yêu thích.&lt;/p&gt;
-&lt;h3&gt;Thông tin sản phẩm:&lt;/h3&gt;
-&lt;p&gt;- Sản phẩm sử dụng nhựa cao cấp đảm bảo an toàn cho bé. &lt;br&gt;- Thích hợp cho bé từ 3 tuổi trở lên.&lt;/p&gt;
-&lt;p&gt;&lt;img style="vertical-align: baseline; display: block; margin-left: auto; margin-right: auto;" src="https://www.mykingdom.com.vn/media/wysiwyg/Long/Line_Robot_bi_n_h_nh_si_u_xe_c_u_h_nh_.png" width="711" height="400"&gt;&lt;/p&gt;
-&lt;p&gt;&lt;br&gt; - Sản phẩm không sử dụng Pin&lt;/p&gt;</t>
   </si>
   <si>
     <t>https://www.mykingdom.com.vn/media/catalog/product/cache/a237138a07ed0dd2cc8a6fa440635ea6/magento/SUPERWINGS/YW720311/YW720311_1.jpg</t>
@@ -446,12 +399,6 @@
     <t>F2159</t>
   </si>
   <si>
-    <t>Các siêu anh hùng Avengers cần những vũ khí mạnh mẽ mới nhất để chống lại những kẻ tấn công từ thiên hà. 
-Khi các mối đe dọa đến với thế giới, trẻ em có thể tưởng tượng chúng sẽ trang bị cho Avengers các vũ khí tương ứng với mỗi "vị khách không mời"! Liệu những vũ khí Mech Strike nâng cao này có đủ giúp Người Khổng Lồ Xanh Hulk tiết kiệm thời gian chiến đấu không?
-Ngoài ra, vũ khí này cũng có thể gắn vào các Mech Strike Avengers khác để sáng tạo ra một trận chiến hoàn toàn mới!
-THU THẬP trọn bộ nhân vật và thiết bị của Marvel Avengers để làm quà tặng tuyệt vời cho các bé trai và bé gái, bao gồm cả nhân vật Black Panther, Captain America và Iron Man!</t>
-  </si>
-  <si>
     <t>https://www.mykingdom.com.vn/media/catalog/product/cache/a237138a07ed0dd2cc8a6fa440635ea6/f/2/f2159_1_.jpg</t>
   </si>
   <si>
@@ -537,14 +484,6 @@
     <t>T6088/RD</t>
   </si>
   <si>
-    <t>&lt;div class="page-header-hgroup col-l-8 col-m-6"&gt;
-&lt;div class="page-title-wrapper complex"&gt;
-&lt;h2 class="page-title"&gt;VECTO Robot tương lai (đỏ)&amp;nbsp;&lt;span data-sheets-value="{&amp;quot;1&amp;quot;:2,&amp;quot;2&amp;quot;:&amp;quot;T6088/RD&amp;quot;}" data-sheets-userformat="{&amp;quot;2&amp;quot;:10623,&amp;quot;3&amp;quot;:{&amp;quot;1&amp;quot;:0,&amp;quot;3&amp;quot;:1},&amp;quot;4&amp;quot;:{&amp;quot;1&amp;quot;:2,&amp;quot;2&amp;quot;:16777215},&amp;quot;5&amp;quot;:{&amp;quot;1&amp;quot;:[{&amp;quot;1&amp;quot;:2,&amp;quot;2&amp;quot;:0,&amp;quot;5&amp;quot;:{&amp;quot;1&amp;quot;:2,&amp;quot;2&amp;quot;:0}},{&amp;quot;1&amp;quot;:0,&amp;quot;2&amp;quot;:0,&amp;quot;3&amp;quot;:3},{&amp;quot;1&amp;quot;:1,&amp;quot;2&amp;quot;:0,&amp;quot;4&amp;quot;:1}]},&amp;quot;6&amp;quot;:{&amp;quot;1&amp;quot;:[{&amp;quot;1&amp;quot;:2,&amp;quot;2&amp;quot;:0,&amp;quot;5&amp;quot;:{&amp;quot;1&amp;quot;:2,&amp;quot;2&amp;quot;:0}},{&amp;quot;1&amp;quot;:0,&amp;quot;2&amp;quot;:0,&amp;quot;3&amp;quot;:3},{&amp;quot;1&amp;quot;:1,&amp;quot;2&amp;quot;:0,&amp;quot;4&amp;quot;:1}]},&amp;quot;7&amp;quot;:{&amp;quot;1&amp;quot;:[{&amp;quot;1&amp;quot;:2,&amp;quot;2&amp;quot;:0,&amp;quot;5&amp;quot;:{&amp;quot;1&amp;quot;:2,&amp;quot;2&amp;quot;:0}},{&amp;quot;1&amp;quot;:0,&amp;quot;2&amp;quot;:0,&amp;quot;3&amp;quot;:3},{&amp;quot;1&amp;quot;:1,&amp;quot;2&amp;quot;:0,&amp;quot;4&amp;quot;:1}]},&amp;quot;8&amp;quot;:{&amp;quot;1&amp;quot;:[{&amp;quot;1&amp;quot;:2,&amp;quot;2&amp;quot;:0,&amp;quot;5&amp;quot;:{&amp;quot;1&amp;quot;:2,&amp;quot;2&amp;quot;:0}},{&amp;quot;1&amp;quot;:0,&amp;quot;2&amp;quot;:0,&amp;quot;3&amp;quot;:3},{&amp;quot;1&amp;quot;:1,&amp;quot;2&amp;quot;:0,&amp;quot;4&amp;quot;:1}]},&amp;quot;9&amp;quot;:1,&amp;quot;11&amp;quot;:4,&amp;quot;14&amp;quot;:{&amp;quot;1&amp;quot;:2,&amp;quot;2&amp;quot;:0},&amp;quot;16&amp;quot;:12}"&gt;T6088/RD&lt;/span&gt;&lt;/h2&gt;
-&lt;/div&gt;
-&lt;/div&gt;
-&lt;p&gt;Đồ Chơi Robot Tương Lai VECTO T6088/RD&amp;nbsp;mang đến cho trẻ những phút giây khám phá thú vị mới. Trẻ có thể tìm hiểu về thế giới xung quanh, vui chơi cùng với tất cả các bạn để thỏa sức khám phá và tìm hiểu.&lt;br&gt;Bộ đồ chơi có nhiều chi tiết giúp bé thoải sức khám phá và lắp ghép các chi tiết, tăng tính năng sáng tạo và tư duy của trẻ ngay từ khi còn nhỏ.&lt;br&gt;Giúp bé nhận diện màu sắc qua các chi tiết mô phỏng thực tế.&lt;br&gt;Bộ đồ chơi có tính tập thể cao, bé có thể cùng chơi với bạn và người thân phát huy khả năng giao tiếp và hoạt ngôn tốt hơn.&lt;br&gt;Bộ đồ chơi được làm từ chất liệu nhựa cao cấp, an toàn đối với sức khỏe của trẻ nhỏ.&lt;br&gt;Chức năng: Bước/ Lướt tới trước, về sau, sang trái phải với hiệu ứng âm thanh Chơi nhạc, nhảy Điều khiển bằng tay Program 50 bước Pin sạc cho robot/ Pin AAA cho remote.&lt;/p&gt;</t>
-  </si>
-  <si>
     <t>https://www.mykingdom.com.vn/media/catalog/product/cache/a237138a07ed0dd2cc8a6fa440635ea6/t/6/t6088___rd_1.jpg</t>
   </si>
   <si>
@@ -558,12 +497,6 @@
   </si>
   <si>
     <t>T6088/BL</t>
-  </si>
-  <si>
-    <t>&lt;h2 class="page-title"&gt;VECTO Robot tương lai (xanh)&amp;nbsp;T6088/BL&lt;/h2&gt;
-&lt;p&gt;VECTO là thương hiệu đồ chơi được nhiều trẻ em yêu thích bởi sự đa dạng và sáng tạo. Tất cả các sản phẩm của Vecto đều được thiết kế tinh xảo, đa dạng về mẫu mã.&lt;br&gt;Robot chiến tương lai (xanh dương) với chức năng bước tới trước, về sau, sang trái phải với hiệu ứng âm thanh chơi nhạc. &lt;br&gt;Sản phẩm không chỉ là món đồ chơi giải trí, mà còn có tác dụng giúp tư duy của bé linh hoạt hơn đồng thời tăng cường được khả năng vận động và phát triển kỹ năng mềm của trẻ, khai phá trí thông minh của trẻ trong việc điều khiển Robot. Đặc biệt được làm từ chất liệu nhựa an toàn tuyệt đối cho sức khỏe của bé, giúp bé thỏa sức sáng tạo và nhận biết được thế giới xung quanh&lt;/p&gt;
-&lt;h3&gt;Thông tin sản phẩm:&lt;/h3&gt;
-&lt;p&gt;Thương hiệu : VECTO&lt;br&gt;Xuất xứ thương hiệu: Việt Nam&lt;br&gt;Xuất xứ: Trung Quốc&lt;br&gt;Độ tuổi: 5+&lt;br&gt;Chất liệu : Nhựa&lt;/p&gt;</t>
   </si>
   <si>
     <t>https://www.mykingdom.com.vn/media/catalog/product/cache/a237138a07ed0dd2cc8a6fa440635ea6/t/6/t6088___bl_1.jpg</t>
@@ -684,25 +617,6 @@
     <t>5088</t>
   </si>
   <si>
-    <t>&lt;div class="page-header-hgroup col-l-8 col-m-6"&gt;
-&lt;div class="page-title-wrapper complex"&gt;
-&lt;h2 class="page-title"&gt;VECTO Robot cảnh sát ROBOCOP&amp;nbsp;&lt;span data-sheets-value="{&amp;quot;1&amp;quot;:3,&amp;quot;3&amp;quot;:5088}" data-sheets-userformat="{&amp;quot;2&amp;quot;:10623,&amp;quot;3&amp;quot;:{&amp;quot;1&amp;quot;:0,&amp;quot;3&amp;quot;:1},&amp;quot;4&amp;quot;:{&amp;quot;1&amp;quot;:2,&amp;quot;2&amp;quot;:16777215},&amp;quot;5&amp;quot;:{&amp;quot;1&amp;quot;:[{&amp;quot;1&amp;quot;:2,&amp;quot;2&amp;quot;:0,&amp;quot;5&amp;quot;:{&amp;quot;1&amp;quot;:2,&amp;quot;2&amp;quot;:0}},{&amp;quot;1&amp;quot;:0,&amp;quot;2&amp;quot;:0,&amp;quot;3&amp;quot;:3},{&amp;quot;1&amp;quot;:1,&amp;quot;2&amp;quot;:0,&amp;quot;4&amp;quot;:1}]},&amp;quot;6&amp;quot;:{&amp;quot;1&amp;quot;:[{&amp;quot;1&amp;quot;:2,&amp;quot;2&amp;quot;:0,&amp;quot;5&amp;quot;:{&amp;quot;1&amp;quot;:2,&amp;quot;2&amp;quot;:0}},{&amp;quot;1&amp;quot;:0,&amp;quot;2&amp;quot;:0,&amp;quot;3&amp;quot;:3},{&amp;quot;1&amp;quot;:1,&amp;quot;2&amp;quot;:0,&amp;quot;4&amp;quot;:1}]},&amp;quot;7&amp;quot;:{&amp;quot;1&amp;quot;:[{&amp;quot;1&amp;quot;:2,&amp;quot;2&amp;quot;:0,&amp;quot;5&amp;quot;:{&amp;quot;1&amp;quot;:2,&amp;quot;2&amp;quot;:0}},{&amp;quot;1&amp;quot;:0,&amp;quot;2&amp;quot;:0,&amp;quot;3&amp;quot;:3},{&amp;quot;1&amp;quot;:1,&amp;quot;2&amp;quot;:0,&amp;quot;4&amp;quot;:1}]},&amp;quot;8&amp;quot;:{&amp;quot;1&amp;quot;:[{&amp;quot;1&amp;quot;:2,&amp;quot;2&amp;quot;:0,&amp;quot;5&amp;quot;:{&amp;quot;1&amp;quot;:2,&amp;quot;2&amp;quot;:0}},{&amp;quot;1&amp;quot;:0,&amp;quot;2&amp;quot;:0,&amp;quot;3&amp;quot;:3},{&amp;quot;1&amp;quot;:1,&amp;quot;2&amp;quot;:0,&amp;quot;4&amp;quot;:1}]},&amp;quot;9&amp;quot;:1,&amp;quot;11&amp;quot;:4,&amp;quot;14&amp;quot;:{&amp;quot;1&amp;quot;:2,&amp;quot;2&amp;quot;:0},&amp;quot;16&amp;quot;:12}"&gt;5088&lt;/span&gt;&lt;/h2&gt;
-&lt;/div&gt;
-&lt;p class="page-title-wrapper complex"&gt;&lt;span data-sheets-value="{&amp;quot;1&amp;quot;:2,&amp;quot;2&amp;quot;:&amp;quot;Bộ đồ chơi lắp ráp xe giúp bé phát triển kỹ năng vận động tinh thông qua các thao tác vặn, mở ốc khi chơi. Ngoài ra, bé còn rèn luyện được tư duy logic, kỹ năng khéo léo khi mày mò lắp ráp hơn 25 mảnh ghép thành 1 chiếc xe hoàn chỉnh. Bộ sản phẩm bao gồm cả vít vặn rất vừa tay cho bé ở độ tuổi preschool, nhựa chơi được trong nhà và ngoài trời/n Với nhiều chủ đề và chức năng khác nhau, hãy sưu tập đủ bộ để có thể giáo dục bé về các phương tiện có thật trong cuộc sống&amp;quot;}" data-sheets-userformat="{&amp;quot;2&amp;quot;:10685,&amp;quot;3&amp;quot;:{&amp;quot;1&amp;quot;:0,&amp;quot;3&amp;quot;:1},&amp;quot;5&amp;quot;:{&amp;quot;1&amp;quot;:[{&amp;quot;1&amp;quot;:2,&amp;quot;2&amp;quot;:0,&amp;quot;5&amp;quot;:{&amp;quot;1&amp;quot;:2,&amp;quot;2&amp;quot;:0}},{&amp;quot;1&amp;quot;:0,&amp;quot;2&amp;quot;:0,&amp;quot;3&amp;quot;:3},{&amp;quot;1&amp;quot;:1,&amp;quot;2&amp;quot;:0,&amp;quot;4&amp;quot;:1}]},&amp;quot;6&amp;quot;:{&amp;quot;1&amp;quot;:[{&amp;quot;1&amp;quot;:2,&amp;quot;2&amp;quot;:0,&amp;quot;5&amp;quot;:{&amp;quot;1&amp;quot;:2,&amp;quot;2&amp;quot;:0}},{&amp;quot;1&amp;quot;:0,&amp;quot;2&amp;quot;:0,&amp;quot;3&amp;quot;:3},{&amp;quot;1&amp;quot;:1,&amp;quot;2&amp;quot;:0,&amp;quot;4&amp;quot;:1}]},&amp;quot;7&amp;quot;:{&amp;quot;1&amp;quot;:[{&amp;quot;1&amp;quot;:2,&amp;quot;2&amp;quot;:0,&amp;quot;5&amp;quot;:{&amp;quot;1&amp;quot;:2,&amp;quot;2&amp;quot;:0}},{&amp;quot;1&amp;quot;:0,&amp;quot;2&amp;quot;:0,&amp;quot;3&amp;quot;:3},{&amp;quot;1&amp;quot;:1,&amp;quot;2&amp;quot;:0,&amp;quot;4&amp;quot;:1}]},&amp;quot;8&amp;quot;:{&amp;quot;1&amp;quot;:[{&amp;quot;1&amp;quot;:2,&amp;quot;2&amp;quot;:0,&amp;quot;5&amp;quot;:{&amp;quot;1&amp;quot;:2,&amp;quot;2&amp;quot;:0}},{&amp;quot;1&amp;quot;:0,&amp;quot;2&amp;quot;:0,&amp;quot;3&amp;quot;:3},{&amp;quot;1&amp;quot;:1,&amp;quot;2&amp;quot;:0,&amp;quot;4&amp;quot;:1}]},&amp;quot;10&amp;quot;:0,&amp;quot;11&amp;quot;:4,&amp;quot;14&amp;quot;:{&amp;quot;1&amp;quot;:3,&amp;quot;3&amp;quot;:1},&amp;quot;16&amp;quot;:12}"&gt;&lt;span data-sheets-value="{&amp;quot;1&amp;quot;:2,&amp;quot;2&amp;quot;:&amp;quot;Bộ đồ chơi lắp ráp xe giúp bé phát triển kỹ năng vận động tinh thông qua các thao tác vặn, mở ốc khi chơi. Ngoài ra, bé còn rèn luyện được tư duy logic, kỹ năng khéo léo khi mày mò lắp ráp hơn 25 mảnh ghép thành 1 chiếc xe hoàn chỉnh. Bộ sản phẩm bao gồm cả vít vặn rất vừa tay cho bé ở độ tuổi preschool, nhựa chơi được trong nhà và ngoài trời/n Với nhiều chủ đề và chức năng khác nhau, hãy sưu tập đủ bộ để có thể giáo dục bé về các phương tiện có thật trong cuộc sống&amp;quot;}" data-sheets-userformat="{&amp;quot;2&amp;quot;:10685,&amp;quot;3&amp;quot;:{&amp;quot;1&amp;quot;:0,&amp;quot;3&amp;quot;:1},&amp;quot;5&amp;quot;:{&amp;quot;1&amp;quot;:[{&amp;quot;1&amp;quot;:2,&amp;quot;2&amp;quot;:0,&amp;quot;5&amp;quot;:{&amp;quot;1&amp;quot;:2,&amp;quot;2&amp;quot;:0}},{&amp;quot;1&amp;quot;:0,&amp;quot;2&amp;quot;:0,&amp;quot;3&amp;quot;:3},{&amp;quot;1&amp;quot;:1,&amp;quot;2&amp;quot;:0,&amp;quot;4&amp;quot;:1}]},&amp;quot;6&amp;quot;:{&amp;quot;1&amp;quot;:[{&amp;quot;1&amp;quot;:2,&amp;quot;2&amp;quot;:0,&amp;quot;5&amp;quot;:{&amp;quot;1&amp;quot;:2,&amp;quot;2&amp;quot;:0}},{&amp;quot;1&amp;quot;:0,&amp;quot;2&amp;quot;:0,&amp;quot;3&amp;quot;:3},{&amp;quot;1&amp;quot;:1,&amp;quot;2&amp;quot;:0,&amp;quot;4&amp;quot;:1}]},&amp;quot;7&amp;quot;:{&amp;quot;1&amp;quot;:[{&amp;quot;1&amp;quot;:2,&amp;quot;2&amp;quot;:0,&amp;quot;5&amp;quot;:{&amp;quot;1&amp;quot;:2,&amp;quot;2&amp;quot;:0}},{&amp;quot;1&amp;quot;:0,&amp;quot;2&amp;quot;:0,&amp;quot;3&amp;quot;:3},{&amp;quot;1&amp;quot;:1,&amp;quot;2&amp;quot;:0,&amp;quot;4&amp;quot;:1}]},&amp;quot;8&amp;quot;:{&amp;quot;1&amp;quot;:[{&amp;quot;1&amp;quot;:2,&amp;quot;2&amp;quot;:0,&amp;quot;5&amp;quot;:{&amp;quot;1&amp;quot;:2,&amp;quot;2&amp;quot;:0}},{&amp;quot;1&amp;quot;:0,&amp;quot;2&amp;quot;:0,&amp;quot;3&amp;quot;:3},{&amp;quot;1&amp;quot;:1,&amp;quot;2&amp;quot;:0,&amp;quot;4&amp;quot;:1}]},&amp;quot;10&amp;quot;:0,&amp;quot;11&amp;quot;:4,&amp;quot;14&amp;quot;:{&amp;quot;1&amp;quot;:3,&amp;quot;3&amp;quot;:1},&amp;quot;16&amp;quot;:12}"&gt;&lt;span&gt;ROBOT CẢNH SÁT ROBOCOP&lt;/span&gt;&lt;br&gt;&lt;span&gt;Dòng Robot điều khiển từ xa với kích thước siêu to. Chú được tích hợp nhiều chức năng thông minh như lập trình trí tuệ lên tới 48 bước, chế độ đi tuần tra, chế độ nhảy múa điêu luyện.&lt;br&gt;&lt;/span&gt;&lt;span&gt;Đặc biệt hơn nữa, bé còn có thể kích hoạt chế độ bắn súng đầy ấn tượng.&lt;/span&gt;&lt;br&gt; Với nhiều chủ đề và chức năng khác nhau, hãy sưu tập đủ bộ để có thể giáo dục bé về các phương tiện có thật trong cuộc sống.&lt;/span&gt;&lt;/span&gt;&lt;/p&gt;
-&lt;h3 class="page-title-wrapper complex"&gt;&lt;span data-sheets-value="{&amp;quot;1&amp;quot;:2,&amp;quot;2&amp;quot;:&amp;quot;Bộ đồ chơi lắp ráp xe giúp bé phát triển kỹ năng vận động tinh thông qua các thao tác vặn, mở ốc khi chơi. Ngoài ra, bé còn rèn luyện được tư duy logic, kỹ năng khéo léo khi mày mò lắp ráp hơn 25 mảnh ghép thành 1 chiếc xe hoàn chỉnh. Bộ sản phẩm bao gồm cả vít vặn rất vừa tay cho bé ở độ tuổi preschool, nhựa chơi được trong nhà và ngoài trời/n Với nhiều chủ đề và chức năng khác nhau, hãy sưu tập đủ bộ để có thể giáo dục bé về các phương tiện có thật trong cuộc sống&amp;quot;}" data-sheets-userformat="{&amp;quot;2&amp;quot;:10685,&amp;quot;3&amp;quot;:{&amp;quot;1&amp;quot;:0,&amp;quot;3&amp;quot;:1},&amp;quot;5&amp;quot;:{&amp;quot;1&amp;quot;:[{&amp;quot;1&amp;quot;:2,&amp;quot;2&amp;quot;:0,&amp;quot;5&amp;quot;:{&amp;quot;1&amp;quot;:2,&amp;quot;2&amp;quot;:0}},{&amp;quot;1&amp;quot;:0,&amp;quot;2&amp;quot;:0,&amp;quot;3&amp;quot;:3},{&amp;quot;1&amp;quot;:1,&amp;quot;2&amp;quot;:0,&amp;quot;4&amp;quot;:1}]},&amp;quot;6&amp;quot;:{&amp;quot;1&amp;quot;:[{&amp;quot;1&amp;quot;:2,&amp;quot;2&amp;quot;:0,&amp;quot;5&amp;quot;:{&amp;quot;1&amp;quot;:2,&amp;quot;2&amp;quot;:0}},{&amp;quot;1&amp;quot;:0,&amp;quot;2&amp;quot;:0,&amp;quot;3&amp;quot;:3},{&amp;quot;1&amp;quot;:1,&amp;quot;2&amp;quot;:0,&amp;quot;4&amp;quot;:1}]},&amp;quot;7&amp;quot;:{&amp;quot;1&amp;quot;:[{&amp;quot;1&amp;quot;:2,&amp;quot;2&amp;quot;:0,&amp;quot;5&amp;quot;:{&amp;quot;1&amp;quot;:2,&amp;quot;2&amp;quot;:0}},{&amp;quot;1&amp;quot;:0,&amp;quot;2&amp;quot;:0,&amp;quot;3&amp;quot;:3},{&amp;quot;1&amp;quot;:1,&amp;quot;2&amp;quot;:0,&amp;quot;4&amp;quot;:1}]},&amp;quot;8&amp;quot;:{&amp;quot;1&amp;quot;:[{&amp;quot;1&amp;quot;:2,&amp;quot;2&amp;quot;:0,&amp;quot;5&amp;quot;:{&amp;quot;1&amp;quot;:2,&amp;quot;2&amp;quot;:0}},{&amp;quot;1&amp;quot;:0,&amp;quot;2&amp;quot;:0,&amp;quot;3&amp;quot;:3},{&amp;quot;1&amp;quot;:1,&amp;quot;2&amp;quot;:0,&amp;quot;4&amp;quot;:1}]},&amp;quot;10&amp;quot;:0,&amp;quot;11&amp;quot;:4,&amp;quot;14&amp;quot;:{&amp;quot;1&amp;quot;:3,&amp;quot;3&amp;quot;:1},&amp;quot;16&amp;quot;:12}"&gt;&lt;span data-sheets-value="{&amp;quot;1&amp;quot;:2,&amp;quot;2&amp;quot;:&amp;quot;Bộ đồ chơi lắp ráp xe giúp bé phát triển kỹ năng vận động tinh thông qua các thao tác vặn, mở ốc khi chơi. Ngoài ra, bé còn rèn luyện được tư duy logic, kỹ năng khéo léo khi mày mò lắp ráp hơn 25 mảnh ghép thành 1 chiếc xe hoàn chỉnh. Bộ sản phẩm bao gồm cả vít vặn rất vừa tay cho bé ở độ tuổi preschool, nhựa chơi được trong nhà và ngoài trời/n Với nhiều chủ đề và chức năng khác nhau, hãy sưu tập đủ bộ để có thể giáo dục bé về các phương tiện có thật trong cuộc sống&amp;quot;}" data-sheets-userformat="{&amp;quot;2&amp;quot;:10685,&amp;quot;3&amp;quot;:{&amp;quot;1&amp;quot;:0,&amp;quot;3&amp;quot;:1},&amp;quot;5&amp;quot;:{&amp;quot;1&amp;quot;:[{&amp;quot;1&amp;quot;:2,&amp;quot;2&amp;quot;:0,&amp;quot;5&amp;quot;:{&amp;quot;1&amp;quot;:2,&amp;quot;2&amp;quot;:0}},{&amp;quot;1&amp;quot;:0,&amp;quot;2&amp;quot;:0,&amp;quot;3&amp;quot;:3},{&amp;quot;1&amp;quot;:1,&amp;quot;2&amp;quot;:0,&amp;quot;4&amp;quot;:1}]},&amp;quot;6&amp;quot;:{&amp;quot;1&amp;quot;:[{&amp;quot;1&amp;quot;:2,&amp;quot;2&amp;quot;:0,&amp;quot;5&amp;quot;:{&amp;quot;1&amp;quot;:2,&amp;quot;2&amp;quot;:0}},{&amp;quot;1&amp;quot;:0,&amp;quot;2&amp;quot;:0,&amp;quot;3&amp;quot;:3},{&amp;quot;1&amp;quot;:1,&amp;quot;2&amp;quot;:0,&amp;quot;4&amp;quot;:1}]},&amp;quot;7&amp;quot;:{&amp;quot;1&amp;quot;:[{&amp;quot;1&amp;quot;:2,&amp;quot;2&amp;quot;:0,&amp;quot;5&amp;quot;:{&amp;quot;1&amp;quot;:2,&amp;quot;2&amp;quot;:0}},{&amp;quot;1&amp;quot;:0,&amp;quot;2&amp;quot;:0,&amp;quot;3&amp;quot;:3},{&amp;quot;1&amp;quot;:1,&amp;quot;2&amp;quot;:0,&amp;quot;4&amp;quot;:1}]},&amp;quot;8&amp;quot;:{&amp;quot;1&amp;quot;:[{&amp;quot;1&amp;quot;:2,&amp;quot;2&amp;quot;:0,&amp;quot;5&amp;quot;:{&amp;quot;1&amp;quot;:2,&amp;quot;2&amp;quot;:0}},{&amp;quot;1&amp;quot;:0,&amp;quot;2&amp;quot;:0,&amp;quot;3&amp;quot;:3},{&amp;quot;1&amp;quot;:1,&amp;quot;2&amp;quot;:0,&amp;quot;4&amp;quot;:1}]},&amp;quot;10&amp;quot;:0,&amp;quot;11&amp;quot;:4,&amp;quot;14&amp;quot;:{&amp;quot;1&amp;quot;:3,&amp;quot;3&amp;quot;:1},&amp;quot;16&amp;quot;:12}"&gt;Thông tin sản phẩm:&lt;/span&gt;&lt;/span&gt;&lt;/h3&gt;
-&lt;p class="page-title-wrapper complex"&gt;&lt;span data-sheets-value="{&amp;quot;1&amp;quot;:2,&amp;quot;2&amp;quot;:&amp;quot;Bộ đồ chơi lắp ráp xe giúp bé phát triển kỹ năng vận động tinh thông qua các thao tác vặn, mở ốc khi chơi. Ngoài ra, bé còn rèn luyện được tư duy logic, kỹ năng khéo léo khi mày mò lắp ráp hơn 25 mảnh ghép thành 1 chiếc xe hoàn chỉnh. Bộ sản phẩm bao gồm cả vít vặn rất vừa tay cho bé ở độ tuổi preschool, nhựa chơi được trong nhà và ngoài trời/n Với nhiều chủ đề và chức năng khác nhau, hãy sưu tập đủ bộ để có thể giáo dục bé về các phương tiện có thật trong cuộc sống&amp;quot;}" data-sheets-userformat="{&amp;quot;2&amp;quot;:10685,&amp;quot;3&amp;quot;:{&amp;quot;1&amp;quot;:0,&amp;quot;3&amp;quot;:1},&amp;quot;5&amp;quot;:{&amp;quot;1&amp;quot;:[{&amp;quot;1&amp;quot;:2,&amp;quot;2&amp;quot;:0,&amp;quot;5&amp;quot;:{&amp;quot;1&amp;quot;:2,&amp;quot;2&amp;quot;:0}},{&amp;quot;1&amp;quot;:0,&amp;quot;2&amp;quot;:0,&amp;quot;3&amp;quot;:3},{&amp;quot;1&amp;quot;:1,&amp;quot;2&amp;quot;:0,&amp;quot;4&amp;quot;:1}]},&amp;quot;6&amp;quot;:{&amp;quot;1&amp;quot;:[{&amp;quot;1&amp;quot;:2,&amp;quot;2&amp;quot;:0,&amp;quot;5&amp;quot;:{&amp;quot;1&amp;quot;:2,&amp;quot;2&amp;quot;:0}},{&amp;quot;1&amp;quot;:0,&amp;quot;2&amp;quot;:0,&amp;quot;3&amp;quot;:3},{&amp;quot;1&amp;quot;:1,&amp;quot;2&amp;quot;:0,&amp;quot;4&amp;quot;:1}]},&amp;quot;7&amp;quot;:{&amp;quot;1&amp;quot;:[{&amp;quot;1&amp;quot;:2,&amp;quot;2&amp;quot;:0,&amp;quot;5&amp;quot;:{&amp;quot;1&amp;quot;:2,&amp;quot;2&amp;quot;:0}},{&amp;quot;1&amp;quot;:0,&amp;quot;2&amp;quot;:0,&amp;quot;3&amp;quot;:3},{&amp;quot;1&amp;quot;:1,&amp;quot;2&amp;quot;:0,&amp;quot;4&amp;quot;:1}]},&amp;quot;8&amp;quot;:{&amp;quot;1&amp;quot;:[{&amp;quot;1&amp;quot;:2,&amp;quot;2&amp;quot;:0,&amp;quot;5&amp;quot;:{&amp;quot;1&amp;quot;:2,&amp;quot;2&amp;quot;:0}},{&amp;quot;1&amp;quot;:0,&amp;quot;2&amp;quot;:0,&amp;quot;3&amp;quot;:3},{&amp;quot;1&amp;quot;:1,&amp;quot;2&amp;quot;:0,&amp;quot;4&amp;quot;:1}]},&amp;quot;10&amp;quot;:0,&amp;quot;11&amp;quot;:4,&amp;quot;14&amp;quot;:{&amp;quot;1&amp;quot;:3,&amp;quot;3&amp;quot;:1},&amp;quot;16&amp;quot;:12}"&gt;&lt;span data-sheets-value="{&amp;quot;1&amp;quot;:2,&amp;quot;2&amp;quot;:&amp;quot;Bộ đồ chơi lắp ráp xe giúp bé phát triển kỹ năng vận động tinh thông qua các thao tác vặn, mở ốc khi chơi. Ngoài ra, bé còn rèn luyện được tư duy logic, kỹ năng khéo léo khi mày mò lắp ráp hơn 25 mảnh ghép thành 1 chiếc xe hoàn chỉnh. Bộ sản phẩm bao gồm cả vít vặn rất vừa tay cho bé ở độ tuổi preschool, nhựa chơi được trong nhà và ngoài trời/n Với nhiều chủ đề và chức năng khác nhau, hãy sưu tập đủ bộ để có thể giáo dục bé về các phương tiện có thật trong cuộc sống&amp;quot;}" data-sheets-userformat="{&amp;quot;2&amp;quot;:10685,&amp;quot;3&amp;quot;:{&amp;quot;1&amp;quot;:0,&amp;quot;3&amp;quot;:1},&amp;quot;5&amp;quot;:{&amp;quot;1&amp;quot;:[{&amp;quot;1&amp;quot;:2,&amp;quot;2&amp;quot;:0,&amp;quot;5&amp;quot;:{&amp;quot;1&amp;quot;:2,&amp;quot;2&amp;quot;:0}},{&amp;quot;1&amp;quot;:0,&amp;quot;2&amp;quot;:0,&amp;quot;3&amp;quot;:3},{&amp;quot;1&amp;quot;:1,&amp;quot;2&amp;quot;:0,&amp;quot;4&amp;quot;:1}]},&amp;quot;6&amp;quot;:{&amp;quot;1&amp;quot;:[{&amp;quot;1&amp;quot;:2,&amp;quot;2&amp;quot;:0,&amp;quot;5&amp;quot;:{&amp;quot;1&amp;quot;:2,&amp;quot;2&amp;quot;:0}},{&amp;quot;1&amp;quot;:0,&amp;quot;2&amp;quot;:0,&amp;quot;3&amp;quot;:3},{&amp;quot;1&amp;quot;:1,&amp;quot;2&amp;quot;:0,&amp;quot;4&amp;quot;:1}]},&amp;quot;7&amp;quot;:{&amp;quot;1&amp;quot;:[{&amp;quot;1&amp;quot;:2,&amp;quot;2&amp;quot;:0,&amp;quot;5&amp;quot;:{&amp;quot;1&amp;quot;:2,&amp;quot;2&amp;quot;:0}},{&amp;quot;1&amp;quot;:0,&amp;quot;2&amp;quot;:0,&amp;quot;3&amp;quot;:3},{&amp;quot;1&amp;quot;:1,&amp;quot;2&amp;quot;:0,&amp;quot;4&amp;quot;:1}]},&amp;quot;8&amp;quot;:{&amp;quot;1&amp;quot;:[{&amp;quot;1&amp;quot;:2,&amp;quot;2&amp;quot;:0,&amp;quot;5&amp;quot;:{&amp;quot;1&amp;quot;:2,&amp;quot;2&amp;quot;:0}},{&amp;quot;1&amp;quot;:0,&amp;quot;2&amp;quot;:0,&amp;quot;3&amp;quot;:3},{&amp;quot;1&amp;quot;:1,&amp;quot;2&amp;quot;:0,&amp;quot;4&amp;quot;:1}]},&amp;quot;10&amp;quot;:0,&amp;quot;11&amp;quot;:4,&amp;quot;14&amp;quot;:{&amp;quot;1&amp;quot;:3,&amp;quot;3&amp;quot;:1},&amp;quot;16&amp;quot;:12}"&gt;&lt;/span&gt;&lt;/span&gt;&lt;/p&gt;
-&lt;ul&gt;
-&lt;li&gt;Thương hiệu: VECTO&lt;/li&gt;
-&lt;li&gt;Xuất xứ thương hiệu: Việt Nam&lt;/li&gt;
-&lt;li&gt;Chất liệu: Nhựa cao cấp&lt;/li&gt;
-&lt;li&gt;Độ tuổi: 4+&lt;/li&gt;
-&lt;li&gt;Giới tính: Bé trai&lt;/li&gt;
-&lt;/ul&gt;
-&lt;p class="page-title-wrapper complex"&gt;&lt;span data-sheets-value="{&amp;quot;1&amp;quot;:2,&amp;quot;2&amp;quot;:&amp;quot;Bộ đồ chơi lắp ráp xe giúp bé phát triển kỹ năng vận động tinh thông qua các thao tác vặn, mở ốc khi chơi. Ngoài ra, bé còn rèn luyện được tư duy logic, kỹ năng khéo léo khi mày mò lắp ráp hơn 25 mảnh ghép thành 1 chiếc xe hoàn chỉnh. Bộ sản phẩm bao gồm cả vít vặn rất vừa tay cho bé ở độ tuổi preschool, nhựa chơi được trong nhà và ngoài trời/n Với nhiều chủ đề và chức năng khác nhau, hãy sưu tập đủ bộ để có thể giáo dục bé về các phương tiện có thật trong cuộc sống&amp;quot;}" data-sheets-userformat="{&amp;quot;2&amp;quot;:10685,&amp;quot;3&amp;quot;:{&amp;quot;1&amp;quot;:0,&amp;quot;3&amp;quot;:1},&amp;quot;5&amp;quot;:{&amp;quot;1&amp;quot;:[{&amp;quot;1&amp;quot;:2,&amp;quot;2&amp;quot;:0,&amp;quot;5&amp;quot;:{&amp;quot;1&amp;quot;:2,&amp;quot;2&amp;quot;:0}},{&amp;quot;1&amp;quot;:0,&amp;quot;2&amp;quot;:0,&amp;quot;3&amp;quot;:3},{&amp;quot;1&amp;quot;:1,&amp;quot;2&amp;quot;:0,&amp;quot;4&amp;quot;:1}]},&amp;quot;6&amp;quot;:{&amp;quot;1&amp;quot;:[{&amp;quot;1&amp;quot;:2,&amp;quot;2&amp;quot;:0,&amp;quot;5&amp;quot;:{&amp;quot;1&amp;quot;:2,&amp;quot;2&amp;quot;:0}},{&amp;quot;1&amp;quot;:0,&amp;quot;2&amp;quot;:0,&amp;quot;3&amp;quot;:3},{&amp;quot;1&amp;quot;:1,&amp;quot;2&amp;quot;:0,&amp;quot;4&amp;quot;:1}]},&amp;quot;7&amp;quot;:{&amp;quot;1&amp;quot;:[{&amp;quot;1&amp;quot;:2,&amp;quot;2&amp;quot;:0,&amp;quot;5&amp;quot;:{&amp;quot;1&amp;quot;:2,&amp;quot;2&amp;quot;:0}},{&amp;quot;1&amp;quot;:0,&amp;quot;2&amp;quot;:0,&amp;quot;3&amp;quot;:3},{&amp;quot;1&amp;quot;:1,&amp;quot;2&amp;quot;:0,&amp;quot;4&amp;quot;:1}]},&amp;quot;8&amp;quot;:{&amp;quot;1&amp;quot;:[{&amp;quot;1&amp;quot;:2,&amp;quot;2&amp;quot;:0,&amp;quot;5&amp;quot;:{&amp;quot;1&amp;quot;:2,&amp;quot;2&amp;quot;:0}},{&amp;quot;1&amp;quot;:0,&amp;quot;2&amp;quot;:0,&amp;quot;3&amp;quot;:3},{&amp;quot;1&amp;quot;:1,&amp;quot;2&amp;quot;:0,&amp;quot;4&amp;quot;:1}]},&amp;quot;10&amp;quot;:0,&amp;quot;11&amp;quot;:4,&amp;quot;14&amp;quot;:{&amp;quot;1&amp;quot;:3,&amp;quot;3&amp;quot;:1},&amp;quot;16&amp;quot;:12}"&gt;&lt;span data-sheets-value="{&amp;quot;1&amp;quot;:2,&amp;quot;2&amp;quot;:&amp;quot;Bộ đồ chơi lắp ráp xe giúp bé phát triển kỹ năng vận động tinh thông qua các thao tác vặn, mở ốc khi chơi. Ngoài ra, bé còn rèn luyện được tư duy logic, kỹ năng khéo léo khi mày mò lắp ráp hơn 25 mảnh ghép thành 1 chiếc xe hoàn chỉnh. Bộ sản phẩm bao gồm cả vít vặn rất vừa tay cho bé ở độ tuổi preschool, nhựa chơi được trong nhà và ngoài trời/n Với nhiều chủ đề và chức năng khác nhau, hãy sưu tập đủ bộ để có thể giáo dục bé về các phương tiện có thật trong cuộc sống&amp;quot;}" data-sheets-userformat="{&amp;quot;2&amp;quot;:10685,&amp;quot;3&amp;quot;:{&amp;quot;1&amp;quot;:0,&amp;quot;3&amp;quot;:1},&amp;quot;5&amp;quot;:{&amp;quot;1&amp;quot;:[{&amp;quot;1&amp;quot;:2,&amp;quot;2&amp;quot;:0,&amp;quot;5&amp;quot;:{&amp;quot;1&amp;quot;:2,&amp;quot;2&amp;quot;:0}},{&amp;quot;1&amp;quot;:0,&amp;quot;2&amp;quot;:0,&amp;quot;3&amp;quot;:3},{&amp;quot;1&amp;quot;:1,&amp;quot;2&amp;quot;:0,&amp;quot;4&amp;quot;:1}]},&amp;quot;6&amp;quot;:{&amp;quot;1&amp;quot;:[{&amp;quot;1&amp;quot;:2,&amp;quot;2&amp;quot;:0,&amp;quot;5&amp;quot;:{&amp;quot;1&amp;quot;:2,&amp;quot;2&amp;quot;:0}},{&amp;quot;1&amp;quot;:0,&amp;quot;2&amp;quot;:0,&amp;quot;3&amp;quot;:3},{&amp;quot;1&amp;quot;:1,&amp;quot;2&amp;quot;:0,&amp;quot;4&amp;quot;:1}]},&amp;quot;7&amp;quot;:{&amp;quot;1&amp;quot;:[{&amp;quot;1&amp;quot;:2,&amp;quot;2&amp;quot;:0,&amp;quot;5&amp;quot;:{&amp;quot;1&amp;quot;:2,&amp;quot;2&amp;quot;:0}},{&amp;quot;1&amp;quot;:0,&amp;quot;2&amp;quot;:0,&amp;quot;3&amp;quot;:3},{&amp;quot;1&amp;quot;:1,&amp;quot;2&amp;quot;:0,&amp;quot;4&amp;quot;:1}]},&amp;quot;8&amp;quot;:{&amp;quot;1&amp;quot;:[{&amp;quot;1&amp;quot;:2,&amp;quot;2&amp;quot;:0,&amp;quot;5&amp;quot;:{&amp;quot;1&amp;quot;:2,&amp;quot;2&amp;quot;:0}},{&amp;quot;1&amp;quot;:0,&amp;quot;2&amp;quot;:0,&amp;quot;3&amp;quot;:3},{&amp;quot;1&amp;quot;:1,&amp;quot;2&amp;quot;:0,&amp;quot;4&amp;quot;:1}]},&amp;quot;10&amp;quot;:0,&amp;quot;11&amp;quot;:4,&amp;quot;14&amp;quot;:{&amp;quot;1&amp;quot;:3,&amp;quot;3&amp;quot;:1},&amp;quot;16&amp;quot;:12}"&gt;&lt;/span&gt;&lt;/span&gt;&lt;/p&gt;
-&lt;/div&gt;
-&lt;div class="page-title-wrapper complex"&gt;&lt;span&gt;VECTO là thương hiệu đồ chơi dành cho bé trai. Được tạo ra để đem đến cho các bé những món đồ chơi an toàn, chất lượng, mang lại thật nhiều niềm vui đồng thời giúp bé phát triển các giác quan, kỹ năng. VECTO có rất nhiều sản phẩm đa dạng được chia thành các chủ đề: xe điều khiển từ xa, robot điều khiển từ xa, đồ chơi bay, đồ chơi lắp ráp, mô hình các phương tiện, xe lửa chạy pin….&lt;/span&gt;&lt;/div&gt;</t>
-  </si>
-  <si>
     <t>https://www.mykingdom.com.vn/media/catalog/product/cache/a237138a07ed0dd2cc8a6fa440635ea6/5/0/5088_1.jpg</t>
   </si>
   <si>
@@ -774,6 +688,98 @@
   </si>
   <si>
     <t>https://www.mykingdom.com.vn/media/catalog/product/cache/a237138a07ed0dd2cc8a6fa440635ea6/7/7/778988245835_20130950_12_inch_set_batmobile_with_figure_m03_gml_product_2.jpg</t>
+  </si>
+  <si>
+    <t>age</t>
+  </si>
+  <si>
+    <t>gender</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Super Wings là bộ phim hoạt hình nổi tiếng đến từ Hàn Quốc, nhận được nhiều sự yêu thích của trẻ em trên toàn thế giới.&lt;/p&gt;
+&lt;p&gt;Robot biến hình kết hợp xe cứu hộ nhỏ - cảnh sát Paul&lt;/p&gt;
+&lt;p&gt;- Biến đổi dễ dàng từ robot cao gần 7 inch thành xe cứu hộ nhỏ qua 3 bước biến hình đơn giản.&lt;br&gt; - Với bánh xe cao su và thang cứu hộ mở rộng tạo cảm giác chân thật khi chơi.&lt;br&gt; - Kích thích tư duy thông qua trò chơi, rèn luyện ngón tay và trí tưởng tượng của bé khi hoá thân vào nhân vật yêu thích.&lt;/p&gt;
+&lt;p&gt;Thông tin sản phẩm:&lt;br&gt; - Sản phẩm sử dụng nhựa cao cấp đảm bảo an toàn cho bé. &lt;br&gt; - Thích hợp cho bé từ 3 tuổi trở lên.&lt;br&gt; - Sản phẩm không sử dụng Pin&lt;/p&gt;
+&lt;p&gt;&lt;img style='vertical-align: baseline; display: block; margin-left: auto; margin-right: auto;' src='https://www.mykingdom.com.vn/media/wysiwyg/Long/Line_Robot_bi_n_h_nh_si_u_xe_c_u_h_nh_.png' width='711' height='400'&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;h2&gt;&lt;span style='font-size: 12px;'&gt;&lt;/span&gt;&lt;/h2&gt;
+&lt;h2&gt;Robot biến hình kết hợp xe cứu hộ nhỏ - Dizzy Lốc Xoáy&lt;/h2&gt;
+&lt;h2&gt;&lt;span style='font-size: 12px;'&gt;Super Wings là bộ phim hoạt hình nổi tiếng đến từ Hàn Quốc, nhận được nhiều sự yêu thích của trẻ em trên toàn thế giới.&lt;/span&gt;&lt;/h2&gt;
+&lt;p&gt;Robot biến hình kết hợp xe cứu hộ nhỏ - Dizzy Lốc Xoáy&lt;/p&gt;
+&lt;p&gt;- Biến đổi dễ dàng từ robot cao gần 7 inch thành xe cứu hộ nhỏ qua 3 bước biến hình đơn giản.&lt;br&gt; - Với bánh xe cao su và thang cứu hộ mở rộng tạo cảm giác chân thật khi chơi.&lt;br&gt; - Kích thích tư duy thông qua trò chơi, rèn luyện ngón tay và trí tưởng tượng của bé khi hoá thân vào nhân vật yêu thích.&lt;/p&gt;
+&lt;h3&gt;Thông tin sản phẩm:&lt;/h3&gt;
+&lt;p&gt;- Sản phẩm sử dụng nhựa cao cấp đảm bảo an toàn cho bé. &lt;br&gt; - Thích hợp cho bé từ 3 tuổi trở lên.&lt;br&gt; - Sản phẩm không sử dụng Pin&lt;/p&gt;
+&lt;p&gt;&lt;img style='vertical-align: baseline; display: block; margin-left: auto; margin-right: auto;' src='https://www.mykingdom.com.vn/media/wysiwyg/Long/Line_Robot_bi_n_h_nh_si_u_xe_c_u_h_nh_.png' width='711' height='400'&gt;&lt;/p&gt;
+&lt;p&gt;&lt;br&gt; - Sản phẩm không sử dụng Pin&lt;/p&gt;
+&lt;table class='MsoNormalTable' style='width: 623px; border-collapse: collapse;' border='0' cellspacing='0' cellpadding='0'&gt;
+&lt;tbody&gt;
+&lt;tr style='mso-yfti-irow: 0; mso-yfti-firstrow: yes; mso-yfti-lastrow: yes; height: 14.25pt;'&gt;
+&lt;td style='width: 364.45pt; border: solid windowtext 1.0pt; border-top: none; mso-border-left-alt: solid windowtext .5pt; mso-border-bottom-alt: solid windowtext .5pt; mso-border-right-alt: solid windowtext .5pt; padding: 0in 5.4pt 0in 5.4pt; height: 14.25pt;' nowrap='nowrap' width='486'&gt;
+&lt;p class='MsoNormal' style='margin-bottom: .0001pt; text-align: justify; line-height: normal;'&gt;&lt;span style='font-size: 10.0pt; font-family: 'Tahoma','sans-serif'; mso-fareast-font-family: 'Times New Roman'; color: black;'&gt;Robot biến hình kết hợp xe cứu hộ nhỏ&lt;span style='mso-spacerun: yes;'&gt;&amp;nbsp; &lt;/span&gt;- Dizzy Lốc Xoáy&lt;/span&gt;&lt;/p&gt;
+&lt;/td&gt;
+&lt;/tr&gt;
+&lt;/tbody&gt;
+&lt;/table&gt;</t>
+  </si>
+  <si>
+    <t>&lt;h2&gt;Robot biến hình kết hợp xe cứu hộ nhỏ - Donnie Thông Minh&lt;/h2&gt;
+&lt;p&gt;Super Wings là bộ phim hoạt hình nổi tiếng đến từ Hàn Quốc, nhận được nhiều sự yêu thích của trẻ em trên toàn thế giới.&lt;/p&gt;
+&lt;p&gt;&lt;/p&gt;
+&lt;p&gt;- Biến đổi dễ dàng từ robot cao gần 7 inch thành xe cứu hộ nhỏ qua 3 bước biến hình đơn giản.&lt;br&gt; - Với bánh xe cao su và thang cứu hộ mở rộng tạo cảm giác chân thật khi chơi.&lt;br&gt; - Kích thích tư duy thông qua trò chơi, rèn luyện ngón tay và trí tưởng tượng của bé khi hoá thân vào nhân vật yêu thích.&lt;/p&gt;
+&lt;h3&gt;Thông tin sản phẩm:&lt;/h3&gt;
+&lt;p&gt;- Sản phẩm sử dụng nhựa cao cấp đảm bảo an toàn cho bé. &lt;br&gt;- Thích hợp cho bé từ 3 tuổi trở lên.&lt;/p&gt;
+&lt;p&gt;&lt;img style='vertical-align: baseline; display: block; margin-left: auto; margin-right: auto;' src='https://www.mykingdom.com.vn/media/wysiwyg/Long/Line_Robot_bi_n_h_nh_si_u_xe_c_u_h_nh_.png' width='711' height='400'&gt;&lt;/p&gt;
+&lt;p&gt;&lt;br&gt; - Sản phẩm không sử dụng Pin&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;h2&gt;ROBOT BIẾN HÌNH KÊT HỢP XE CỨU HỘ NHỎ JETT TIA CHỚP&lt;/h2&gt;
+&lt;p&gt;Super Wings là bộ phim hoạt hình nổi tiếng đến từ Hàn Quốc, nhận được nhiều sự yêu thích của trẻ em trên toàn thế giới.&lt;/p&gt;
+&lt;p&gt;Robot biến hình kết hợp xe cứu hộ nhỏ - Jett Tia Chớp&lt;/p&gt;
+&lt;p&gt;- Biến đổi dễ dàng từ robot cao gần 7 inch thành xe cứu hộ nhỏ qua 3 bước biến hình đơn giản.&lt;br&gt; - Với bánh xe cao su và thang cứu hộ mở rộng tạo cảm giác chân thật khi chơi.&lt;br&gt; - Kích thích tư duy thông qua trò chơi, rèn luyện ngón tay và trí tưởng tượng của bé khi hoá thân vào nhân vật yêu thích.&lt;/p&gt;
+&lt;h3&gt;Thông tin sản phẩm:&lt;/h3&gt;
+&lt;p&gt;- Sản phẩm sử dụng nhựa cao cấp đảm bảo an toàn cho bé. &lt;br&gt;- Thích hợp cho bé từ 3 tuổi trở lên.&lt;/p&gt;
+&lt;p&gt;&lt;img style='vertical-align: baseline; display: block; margin-left: auto; margin-right: auto;' src='https://www.mykingdom.com.vn/media/wysiwyg/Long/Line_Robot_bi_n_h_nh_si_u_xe_c_u_h_nh_.png' width='711' height='400'&gt;&lt;/p&gt;
+&lt;p&gt;&lt;br&gt; - Sản phẩm không sử dụng Pin&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>Các siêu anh hùng Avengers cần những vũ khí mạnh mẽ mới nhất để chống lại những kẻ tấn công từ thiên hà. 
+Khi các mối đe dọa đến với thế giới, trẻ em có thể tưởng tượng chúng sẽ trang bị cho Avengers các vũ khí tương ứng với mỗi 'vị khách không mời'! Liệu những vũ khí Mech Strike nâng cao này có đủ giúp Người Khổng Lồ Xanh Hulk tiết kiệm thời gian chiến đấu không?
+Ngoài ra, vũ khí này cũng có thể gắn vào các Mech Strike Avengers khác để sáng tạo ra một trận chiến hoàn toàn mới!
+THU THẬP trọn bộ nhân vật và thiết bị của Marvel Avengers để làm quà tặng tuyệt vời cho các bé trai và bé gái, bao gồm cả nhân vật Black Panther, Captain America và Iron Man!</t>
+  </si>
+  <si>
+    <t>&lt;div class='page-header-hgroup col-l-8 col-m-6'&gt;
+&lt;div class='page-title-wrapper complex'&gt;
+&lt;h2 class='page-title'&gt;VECTO Robot tương lai (đỏ)&amp;nbsp;&lt;span data-sheets-value='{&amp;quot;1&amp;quot;:2,&amp;quot;2&amp;quot;:&amp;quot;T6088/RD&amp;quot;}' data-sheets-userformat='{&amp;quot;2&amp;quot;:10623,&amp;quot;3&amp;quot;:{&amp;quot;1&amp;quot;:0,&amp;quot;3&amp;quot;:1},&amp;quot;4&amp;quot;:{&amp;quot;1&amp;quot;:2,&amp;quot;2&amp;quot;:16777215},&amp;quot;5&amp;quot;:{&amp;quot;1&amp;quot;:[{&amp;quot;1&amp;quot;:2,&amp;quot;2&amp;quot;:0,&amp;quot;5&amp;quot;:{&amp;quot;1&amp;quot;:2,&amp;quot;2&amp;quot;:0}},{&amp;quot;1&amp;quot;:0,&amp;quot;2&amp;quot;:0,&amp;quot;3&amp;quot;:3},{&amp;quot;1&amp;quot;:1,&amp;quot;2&amp;quot;:0,&amp;quot;4&amp;quot;:1}]},&amp;quot;6&amp;quot;:{&amp;quot;1&amp;quot;:[{&amp;quot;1&amp;quot;:2,&amp;quot;2&amp;quot;:0,&amp;quot;5&amp;quot;:{&amp;quot;1&amp;quot;:2,&amp;quot;2&amp;quot;:0}},{&amp;quot;1&amp;quot;:0,&amp;quot;2&amp;quot;:0,&amp;quot;3&amp;quot;:3},{&amp;quot;1&amp;quot;:1,&amp;quot;2&amp;quot;:0,&amp;quot;4&amp;quot;:1}]},&amp;quot;7&amp;quot;:{&amp;quot;1&amp;quot;:[{&amp;quot;1&amp;quot;:2,&amp;quot;2&amp;quot;:0,&amp;quot;5&amp;quot;:{&amp;quot;1&amp;quot;:2,&amp;quot;2&amp;quot;:0}},{&amp;quot;1&amp;quot;:0,&amp;quot;2&amp;quot;:0,&amp;quot;3&amp;quot;:3},{&amp;quot;1&amp;quot;:1,&amp;quot;2&amp;quot;:0,&amp;quot;4&amp;quot;:1}]},&amp;quot;8&amp;quot;:{&amp;quot;1&amp;quot;:[{&amp;quot;1&amp;quot;:2,&amp;quot;2&amp;quot;:0,&amp;quot;5&amp;quot;:{&amp;quot;1&amp;quot;:2,&amp;quot;2&amp;quot;:0}},{&amp;quot;1&amp;quot;:0,&amp;quot;2&amp;quot;:0,&amp;quot;3&amp;quot;:3},{&amp;quot;1&amp;quot;:1,&amp;quot;2&amp;quot;:0,&amp;quot;4&amp;quot;:1}]},&amp;quot;9&amp;quot;:1,&amp;quot;11&amp;quot;:4,&amp;quot;14&amp;quot;:{&amp;quot;1&amp;quot;:2,&amp;quot;2&amp;quot;:0},&amp;quot;16&amp;quot;:12}'&gt;T6088/RD&lt;/span&gt;&lt;/h2&gt;
+&lt;/div&gt;
+&lt;/div&gt;
+&lt;p&gt;Đồ Chơi Robot Tương Lai VECTO T6088/RD&amp;nbsp;mang đến cho trẻ những phút giây khám phá thú vị mới. Trẻ có thể tìm hiểu về thế giới xung quanh, vui chơi cùng với tất cả các bạn để thỏa sức khám phá và tìm hiểu.&lt;br&gt;Bộ đồ chơi có nhiều chi tiết giúp bé thoải sức khám phá và lắp ghép các chi tiết, tăng tính năng sáng tạo và tư duy của trẻ ngay từ khi còn nhỏ.&lt;br&gt;Giúp bé nhận diện màu sắc qua các chi tiết mô phỏng thực tế.&lt;br&gt;Bộ đồ chơi có tính tập thể cao, bé có thể cùng chơi với bạn và người thân phát huy khả năng giao tiếp và hoạt ngôn tốt hơn.&lt;br&gt;Bộ đồ chơi được làm từ chất liệu nhựa cao cấp, an toàn đối với sức khỏe của trẻ nhỏ.&lt;br&gt;Chức năng: Bước/ Lướt tới trước, về sau, sang trái phải với hiệu ứng âm thanh Chơi nhạc, nhảy Điều khiển bằng tay Program 50 bước Pin sạc cho robot/ Pin AAA cho remote.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;h2 class='page-title'&gt;VECTO Robot tương lai (xanh)&amp;nbsp;T6088/BL&lt;/h2&gt;
+&lt;p&gt;VECTO là thương hiệu đồ chơi được nhiều trẻ em yêu thích bởi sự đa dạng và sáng tạo. Tất cả các sản phẩm của Vecto đều được thiết kế tinh xảo, đa dạng về mẫu mã.&lt;br&gt;Robot chiến tương lai (xanh dương) với chức năng bước tới trước, về sau, sang trái phải với hiệu ứng âm thanh chơi nhạc. &lt;br&gt;Sản phẩm không chỉ là món đồ chơi giải trí, mà còn có tác dụng giúp tư duy của bé linh hoạt hơn đồng thời tăng cường được khả năng vận động và phát triển kỹ năng mềm của trẻ, khai phá trí thông minh của trẻ trong việc điều khiển Robot. Đặc biệt được làm từ chất liệu nhựa an toàn tuyệt đối cho sức khỏe của bé, giúp bé thỏa sức sáng tạo và nhận biết được thế giới xung quanh&lt;/p&gt;
+&lt;h3&gt;Thông tin sản phẩm:&lt;/h3&gt;
+&lt;p&gt;Thương hiệu : VECTO&lt;br&gt;Xuất xứ thương hiệu: Việt Nam&lt;br&gt;Xuất xứ: Trung Quốc&lt;br&gt;Độ tuổi: 5+&lt;br&gt;Chất liệu : Nhựa&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;div class='page-header-hgroup col-l-8 col-m-6'&gt;
+&lt;div class='page-title-wrapper complex'&gt;
+&lt;h2 class='page-title'&gt;VECTO Robot cảnh sát ROBOCOP&amp;nbsp;&lt;span data-sheets-value='{&amp;quot;1&amp;quot;:3,&amp;quot;3&amp;quot;:5088}' data-sheets-userformat='{&amp;quot;2&amp;quot;:10623,&amp;quot;3&amp;quot;:{&amp;quot;1&amp;quot;:0,&amp;quot;3&amp;quot;:1},&amp;quot;4&amp;quot;:{&amp;quot;1&amp;quot;:2,&amp;quot;2&amp;quot;:16777215},&amp;quot;5&amp;quot;:{&amp;quot;1&amp;quot;:[{&amp;quot;1&amp;quot;:2,&amp;quot;2&amp;quot;:0,&amp;quot;5&amp;quot;:{&amp;quot;1&amp;quot;:2,&amp;quot;2&amp;quot;:0}},{&amp;quot;1&amp;quot;:0,&amp;quot;2&amp;quot;:0,&amp;quot;3&amp;quot;:3},{&amp;quot;1&amp;quot;:1,&amp;quot;2&amp;quot;:0,&amp;quot;4&amp;quot;:1}]},&amp;quot;6&amp;quot;:{&amp;quot;1&amp;quot;:[{&amp;quot;1&amp;quot;:2,&amp;quot;2&amp;quot;:0,&amp;quot;5&amp;quot;:{&amp;quot;1&amp;quot;:2,&amp;quot;2&amp;quot;:0}},{&amp;quot;1&amp;quot;:0,&amp;quot;2&amp;quot;:0,&amp;quot;3&amp;quot;:3},{&amp;quot;1&amp;quot;:1,&amp;quot;2&amp;quot;:0,&amp;quot;4&amp;quot;:1}]},&amp;quot;7&amp;quot;:{&amp;quot;1&amp;quot;:[{&amp;quot;1&amp;quot;:2,&amp;quot;2&amp;quot;:0,&amp;quot;5&amp;quot;:{&amp;quot;1&amp;quot;:2,&amp;quot;2&amp;quot;:0}},{&amp;quot;1&amp;quot;:0,&amp;quot;2&amp;quot;:0,&amp;quot;3&amp;quot;:3},{&amp;quot;1&amp;quot;:1,&amp;quot;2&amp;quot;:0,&amp;quot;4&amp;quot;:1}]},&amp;quot;8&amp;quot;:{&amp;quot;1&amp;quot;:[{&amp;quot;1&amp;quot;:2,&amp;quot;2&amp;quot;:0,&amp;quot;5&amp;quot;:{&amp;quot;1&amp;quot;:2,&amp;quot;2&amp;quot;:0}},{&amp;quot;1&amp;quot;:0,&amp;quot;2&amp;quot;:0,&amp;quot;3&amp;quot;:3},{&amp;quot;1&amp;quot;:1,&amp;quot;2&amp;quot;:0,&amp;quot;4&amp;quot;:1}]},&amp;quot;9&amp;quot;:1,&amp;quot;11&amp;quot;:4,&amp;quot;14&amp;quot;:{&amp;quot;1&amp;quot;:2,&amp;quot;2&amp;quot;:0},&amp;quot;16&amp;quot;:12}'&gt;5088&lt;/span&gt;&lt;/h2&gt;
+&lt;/div&gt;
+&lt;p class='page-title-wrapper complex'&gt;&lt;span data-sheets-value='{&amp;quot;1&amp;quot;:2,&amp;quot;2&amp;quot;:&amp;quot;Bộ đồ chơi lắp ráp xe giúp bé phát triển kỹ năng vận động tinh thông qua các thao tác vặn, mở ốc khi chơi. Ngoài ra, bé còn rèn luyện được tư duy logic, kỹ năng khéo léo khi mày mò lắp ráp hơn 25 mảnh ghép thành 1 chiếc xe hoàn chỉnh. Bộ sản phẩm bao gồm cả vít vặn rất vừa tay cho bé ở độ tuổi preschool, nhựa chơi được trong nhà và ngoài trời/n Với nhiều chủ đề và chức năng khác nhau, hãy sưu tập đủ bộ để có thể giáo dục bé về các phương tiện có thật trong cuộc sống&amp;quot;}' data-sheets-userformat='{&amp;quot;2&amp;quot;:10685,&amp;quot;3&amp;quot;:{&amp;quot;1&amp;quot;:0,&amp;quot;3&amp;quot;:1},&amp;quot;5&amp;quot;:{&amp;quot;1&amp;quot;:[{&amp;quot;1&amp;quot;:2,&amp;quot;2&amp;quot;:0,&amp;quot;5&amp;quot;:{&amp;quot;1&amp;quot;:2,&amp;quot;2&amp;quot;:0}},{&amp;quot;1&amp;quot;:0,&amp;quot;2&amp;quot;:0,&amp;quot;3&amp;quot;:3},{&amp;quot;1&amp;quot;:1,&amp;quot;2&amp;quot;:0,&amp;quot;4&amp;quot;:1}]},&amp;quot;6&amp;quot;:{&amp;quot;1&amp;quot;:[{&amp;quot;1&amp;quot;:2,&amp;quot;2&amp;quot;:0,&amp;quot;5&amp;quot;:{&amp;quot;1&amp;quot;:2,&amp;quot;2&amp;quot;:0}},{&amp;quot;1&amp;quot;:0,&amp;quot;2&amp;quot;:0,&amp;quot;3&amp;quot;:3},{&amp;quot;1&amp;quot;:1,&amp;quot;2&amp;quot;:0,&amp;quot;4&amp;quot;:1}]},&amp;quot;7&amp;quot;:{&amp;quot;1&amp;quot;:[{&amp;quot;1&amp;quot;:2,&amp;quot;2&amp;quot;:0,&amp;quot;5&amp;quot;:{&amp;quot;1&amp;quot;:2,&amp;quot;2&amp;quot;:0}},{&amp;quot;1&amp;quot;:0,&amp;quot;2&amp;quot;:0,&amp;quot;3&amp;quot;:3},{&amp;quot;1&amp;quot;:1,&amp;quot;2&amp;quot;:0,&amp;quot;4&amp;quot;:1}]},&amp;quot;8&amp;quot;:{&amp;quot;1&amp;quot;:[{&amp;quot;1&amp;quot;:2,&amp;quot;2&amp;quot;:0,&amp;quot;5&amp;quot;:{&amp;quot;1&amp;quot;:2,&amp;quot;2&amp;quot;:0}},{&amp;quot;1&amp;quot;:0,&amp;quot;2&amp;quot;:0,&amp;quot;3&amp;quot;:3},{&amp;quot;1&amp;quot;:1,&amp;quot;2&amp;quot;:0,&amp;quot;4&amp;quot;:1}]},&amp;quot;10&amp;quot;:0,&amp;quot;11&amp;quot;:4,&amp;quot;14&amp;quot;:{&amp;quot;1&amp;quot;:3,&amp;quot;3&amp;quot;:1},&amp;quot;16&amp;quot;:12}'&gt;&lt;span data-sheets-value='{&amp;quot;1&amp;quot;:2,&amp;quot;2&amp;quot;:&amp;quot;Bộ đồ chơi lắp ráp xe giúp bé phát triển kỹ năng vận động tinh thông qua các thao tác vặn, mở ốc khi chơi. Ngoài ra, bé còn rèn luyện được tư duy logic, kỹ năng khéo léo khi mày mò lắp ráp hơn 25 mảnh ghép thành 1 chiếc xe hoàn chỉnh. Bộ sản phẩm bao gồm cả vít vặn rất vừa tay cho bé ở độ tuổi preschool, nhựa chơi được trong nhà và ngoài trời/n Với nhiều chủ đề và chức năng khác nhau, hãy sưu tập đủ bộ để có thể giáo dục bé về các phương tiện có thật trong cuộc sống&amp;quot;}' data-sheets-userformat='{&amp;quot;2&amp;quot;:10685,&amp;quot;3&amp;quot;:{&amp;quot;1&amp;quot;:0,&amp;quot;3&amp;quot;:1},&amp;quot;5&amp;quot;:{&amp;quot;1&amp;quot;:[{&amp;quot;1&amp;quot;:2,&amp;quot;2&amp;quot;:0,&amp;quot;5&amp;quot;:{&amp;quot;1&amp;quot;:2,&amp;quot;2&amp;quot;:0}},{&amp;quot;1&amp;quot;:0,&amp;quot;2&amp;quot;:0,&amp;quot;3&amp;quot;:3},{&amp;quot;1&amp;quot;:1,&amp;quot;2&amp;quot;:0,&amp;quot;4&amp;quot;:1}]},&amp;quot;6&amp;quot;:{&amp;quot;1&amp;quot;:[{&amp;quot;1&amp;quot;:2,&amp;quot;2&amp;quot;:0,&amp;quot;5&amp;quot;:{&amp;quot;1&amp;quot;:2,&amp;quot;2&amp;quot;:0}},{&amp;quot;1&amp;quot;:0,&amp;quot;2&amp;quot;:0,&amp;quot;3&amp;quot;:3},{&amp;quot;1&amp;quot;:1,&amp;quot;2&amp;quot;:0,&amp;quot;4&amp;quot;:1}]},&amp;quot;7&amp;quot;:{&amp;quot;1&amp;quot;:[{&amp;quot;1&amp;quot;:2,&amp;quot;2&amp;quot;:0,&amp;quot;5&amp;quot;:{&amp;quot;1&amp;quot;:2,&amp;quot;2&amp;quot;:0}},{&amp;quot;1&amp;quot;:0,&amp;quot;2&amp;quot;:0,&amp;quot;3&amp;quot;:3},{&amp;quot;1&amp;quot;:1,&amp;quot;2&amp;quot;:0,&amp;quot;4&amp;quot;:1}]},&amp;quot;8&amp;quot;:{&amp;quot;1&amp;quot;:[{&amp;quot;1&amp;quot;:2,&amp;quot;2&amp;quot;:0,&amp;quot;5&amp;quot;:{&amp;quot;1&amp;quot;:2,&amp;quot;2&amp;quot;:0}},{&amp;quot;1&amp;quot;:0,&amp;quot;2&amp;quot;:0,&amp;quot;3&amp;quot;:3},{&amp;quot;1&amp;quot;:1,&amp;quot;2&amp;quot;:0,&amp;quot;4&amp;quot;:1}]},&amp;quot;10&amp;quot;:0,&amp;quot;11&amp;quot;:4,&amp;quot;14&amp;quot;:{&amp;quot;1&amp;quot;:3,&amp;quot;3&amp;quot;:1},&amp;quot;16&amp;quot;:12}'&gt;&lt;span&gt;ROBOT CẢNH SÁT ROBOCOP&lt;/span&gt;&lt;br&gt;&lt;span&gt;Dòng Robot điều khiển từ xa với kích thước siêu to. Chú được tích hợp nhiều chức năng thông minh như lập trình trí tuệ lên tới 48 bước, chế độ đi tuần tra, chế độ nhảy múa điêu luyện.&lt;br&gt;&lt;/span&gt;&lt;span&gt;Đặc biệt hơn nữa, bé còn có thể kích hoạt chế độ bắn súng đầy ấn tượng.&lt;/span&gt;&lt;br&gt; Với nhiều chủ đề và chức năng khác nhau, hãy sưu tập đủ bộ để có thể giáo dục bé về các phương tiện có thật trong cuộc sống.&lt;/span&gt;&lt;/span&gt;&lt;/p&gt;
+&lt;h3 class='page-title-wrapper complex'&gt;&lt;span data-sheets-value='{&amp;quot;1&amp;quot;:2,&amp;quot;2&amp;quot;:&amp;quot;Bộ đồ chơi lắp ráp xe giúp bé phát triển kỹ năng vận động tinh thông qua các thao tác vặn, mở ốc khi chơi. Ngoài ra, bé còn rèn luyện được tư duy logic, kỹ năng khéo léo khi mày mò lắp ráp hơn 25 mảnh ghép thành 1 chiếc xe hoàn chỉnh. Bộ sản phẩm bao gồm cả vít vặn rất vừa tay cho bé ở độ tuổi preschool, nhựa chơi được trong nhà và ngoài trời/n Với nhiều chủ đề và chức năng khác nhau, hãy sưu tập đủ bộ để có thể giáo dục bé về các phương tiện có thật trong cuộc sống&amp;quot;}' data-sheets-userformat='{&amp;quot;2&amp;quot;:10685,&amp;quot;3&amp;quot;:{&amp;quot;1&amp;quot;:0,&amp;quot;3&amp;quot;:1},&amp;quot;5&amp;quot;:{&amp;quot;1&amp;quot;:[{&amp;quot;1&amp;quot;:2,&amp;quot;2&amp;quot;:0,&amp;quot;5&amp;quot;:{&amp;quot;1&amp;quot;:2,&amp;quot;2&amp;quot;:0}},{&amp;quot;1&amp;quot;:0,&amp;quot;2&amp;quot;:0,&amp;quot;3&amp;quot;:3},{&amp;quot;1&amp;quot;:1,&amp;quot;2&amp;quot;:0,&amp;quot;4&amp;quot;:1}]},&amp;quot;6&amp;quot;:{&amp;quot;1&amp;quot;:[{&amp;quot;1&amp;quot;:2,&amp;quot;2&amp;quot;:0,&amp;quot;5&amp;quot;:{&amp;quot;1&amp;quot;:2,&amp;quot;2&amp;quot;:0}},{&amp;quot;1&amp;quot;:0,&amp;quot;2&amp;quot;:0,&amp;quot;3&amp;quot;:3},{&amp;quot;1&amp;quot;:1,&amp;quot;2&amp;quot;:0,&amp;quot;4&amp;quot;:1}]},&amp;quot;7&amp;quot;:{&amp;quot;1&amp;quot;:[{&amp;quot;1&amp;quot;:2,&amp;quot;2&amp;quot;:0,&amp;quot;5&amp;quot;:{&amp;quot;1&amp;quot;:2,&amp;quot;2&amp;quot;:0}},{&amp;quot;1&amp;quot;:0,&amp;quot;2&amp;quot;:0,&amp;quot;3&amp;quot;:3},{&amp;quot;1&amp;quot;:1,&amp;quot;2&amp;quot;:0,&amp;quot;4&amp;quot;:1}]},&amp;quot;8&amp;quot;:{&amp;quot;1&amp;quot;:[{&amp;quot;1&amp;quot;:2,&amp;quot;2&amp;quot;:0,&amp;quot;5&amp;quot;:{&amp;quot;1&amp;quot;:2,&amp;quot;2&amp;quot;:0}},{&amp;quot;1&amp;quot;:0,&amp;quot;2&amp;quot;:0,&amp;quot;3&amp;quot;:3},{&amp;quot;1&amp;quot;:1,&amp;quot;2&amp;quot;:0,&amp;quot;4&amp;quot;:1}]},&amp;quot;10&amp;quot;:0,&amp;quot;11&amp;quot;:4,&amp;quot;14&amp;quot;:{&amp;quot;1&amp;quot;:3,&amp;quot;3&amp;quot;:1},&amp;quot;16&amp;quot;:12}'&gt;&lt;span data-sheets-value='{&amp;quot;1&amp;quot;:2,&amp;quot;2&amp;quot;:&amp;quot;Bộ đồ chơi lắp ráp xe giúp bé phát triển kỹ năng vận động tinh thông qua các thao tác vặn, mở ốc khi chơi. Ngoài ra, bé còn rèn luyện được tư duy logic, kỹ năng khéo léo khi mày mò lắp ráp hơn 25 mảnh ghép thành 1 chiếc xe hoàn chỉnh. Bộ sản phẩm bao gồm cả vít vặn rất vừa tay cho bé ở độ tuổi preschool, nhựa chơi được trong nhà và ngoài trời/n Với nhiều chủ đề và chức năng khác nhau, hãy sưu tập đủ bộ để có thể giáo dục bé về các phương tiện có thật trong cuộc sống&amp;quot;}' data-sheets-userformat='{&amp;quot;2&amp;quot;:10685,&amp;quot;3&amp;quot;:{&amp;quot;1&amp;quot;:0,&amp;quot;3&amp;quot;:1},&amp;quot;5&amp;quot;:{&amp;quot;1&amp;quot;:[{&amp;quot;1&amp;quot;:2,&amp;quot;2&amp;quot;:0,&amp;quot;5&amp;quot;:{&amp;quot;1&amp;quot;:2,&amp;quot;2&amp;quot;:0}},{&amp;quot;1&amp;quot;:0,&amp;quot;2&amp;quot;:0,&amp;quot;3&amp;quot;:3},{&amp;quot;1&amp;quot;:1,&amp;quot;2&amp;quot;:0,&amp;quot;4&amp;quot;:1}]},&amp;quot;6&amp;quot;:{&amp;quot;1&amp;quot;:[{&amp;quot;1&amp;quot;:2,&amp;quot;2&amp;quot;:0,&amp;quot;5&amp;quot;:{&amp;quot;1&amp;quot;:2,&amp;quot;2&amp;quot;:0}},{&amp;quot;1&amp;quot;:0,&amp;quot;2&amp;quot;:0,&amp;quot;3&amp;quot;:3},{&amp;quot;1&amp;quot;:1,&amp;quot;2&amp;quot;:0,&amp;quot;4&amp;quot;:1}]},&amp;quot;7&amp;quot;:{&amp;quot;1&amp;quot;:[{&amp;quot;1&amp;quot;:2,&amp;quot;2&amp;quot;:0,&amp;quot;5&amp;quot;:{&amp;quot;1&amp;quot;:2,&amp;quot;2&amp;quot;:0}},{&amp;quot;1&amp;quot;:0,&amp;quot;2&amp;quot;:0,&amp;quot;3&amp;quot;:3},{&amp;quot;1&amp;quot;:1,&amp;quot;2&amp;quot;:0,&amp;quot;4&amp;quot;:1}]},&amp;quot;8&amp;quot;:{&amp;quot;1&amp;quot;:[{&amp;quot;1&amp;quot;:2,&amp;quot;2&amp;quot;:0,&amp;quot;5&amp;quot;:{&amp;quot;1&amp;quot;:2,&amp;quot;2&amp;quot;:0}},{&amp;quot;1&amp;quot;:0,&amp;quot;2&amp;quot;:0,&amp;quot;3&amp;quot;:3},{&amp;quot;1&amp;quot;:1,&amp;quot;2&amp;quot;:0,&amp;quot;4&amp;quot;:1}]},&amp;quot;10&amp;quot;:0,&amp;quot;11&amp;quot;:4,&amp;quot;14&amp;quot;:{&amp;quot;1&amp;quot;:3,&amp;quot;3&amp;quot;:1},&amp;quot;16&amp;quot;:12}'&gt;Thông tin sản phẩm:&lt;/span&gt;&lt;/span&gt;&lt;/h3&gt;
+&lt;p class='page-title-wrapper complex'&gt;&lt;span data-sheets-value='{&amp;quot;1&amp;quot;:2,&amp;quot;2&amp;quot;:&amp;quot;Bộ đồ chơi lắp ráp xe giúp bé phát triển kỹ năng vận động tinh thông qua các thao tác vặn, mở ốc khi chơi. Ngoài ra, bé còn rèn luyện được tư duy logic, kỹ năng khéo léo khi mày mò lắp ráp hơn 25 mảnh ghép thành 1 chiếc xe hoàn chỉnh. Bộ sản phẩm bao gồm cả vít vặn rất vừa tay cho bé ở độ tuổi preschool, nhựa chơi được trong nhà và ngoài trời/n Với nhiều chủ đề và chức năng khác nhau, hãy sưu tập đủ bộ để có thể giáo dục bé về các phương tiện có thật trong cuộc sống&amp;quot;}' data-sheets-userformat='{&amp;quot;2&amp;quot;:10685,&amp;quot;3&amp;quot;:{&amp;quot;1&amp;quot;:0,&amp;quot;3&amp;quot;:1},&amp;quot;5&amp;quot;:{&amp;quot;1&amp;quot;:[{&amp;quot;1&amp;quot;:2,&amp;quot;2&amp;quot;:0,&amp;quot;5&amp;quot;:{&amp;quot;1&amp;quot;:2,&amp;quot;2&amp;quot;:0}},{&amp;quot;1&amp;quot;:0,&amp;quot;2&amp;quot;:0,&amp;quot;3&amp;quot;:3},{&amp;quot;1&amp;quot;:1,&amp;quot;2&amp;quot;:0,&amp;quot;4&amp;quot;:1}]},&amp;quot;6&amp;quot;:{&amp;quot;1&amp;quot;:[{&amp;quot;1&amp;quot;:2,&amp;quot;2&amp;quot;:0,&amp;quot;5&amp;quot;:{&amp;quot;1&amp;quot;:2,&amp;quot;2&amp;quot;:0}},{&amp;quot;1&amp;quot;:0,&amp;quot;2&amp;quot;:0,&amp;quot;3&amp;quot;:3},{&amp;quot;1&amp;quot;:1,&amp;quot;2&amp;quot;:0,&amp;quot;4&amp;quot;:1}]},&amp;quot;7&amp;quot;:{&amp;quot;1&amp;quot;:[{&amp;quot;1&amp;quot;:2,&amp;quot;2&amp;quot;:0,&amp;quot;5&amp;quot;:{&amp;quot;1&amp;quot;:2,&amp;quot;2&amp;quot;:0}},{&amp;quot;1&amp;quot;:0,&amp;quot;2&amp;quot;:0,&amp;quot;3&amp;quot;:3},{&amp;quot;1&amp;quot;:1,&amp;quot;2&amp;quot;:0,&amp;quot;4&amp;quot;:1}]},&amp;quot;8&amp;quot;:{&amp;quot;1&amp;quot;:[{&amp;quot;1&amp;quot;:2,&amp;quot;2&amp;quot;:0,&amp;quot;5&amp;quot;:{&amp;quot;1&amp;quot;:2,&amp;quot;2&amp;quot;:0}},{&amp;quot;1&amp;quot;:0,&amp;quot;2&amp;quot;:0,&amp;quot;3&amp;quot;:3},{&amp;quot;1&amp;quot;:1,&amp;quot;2&amp;quot;:0,&amp;quot;4&amp;quot;:1}]},&amp;quot;10&amp;quot;:0,&amp;quot;11&amp;quot;:4,&amp;quot;14&amp;quot;:{&amp;quot;1&amp;quot;:3,&amp;quot;3&amp;quot;:1},&amp;quot;16&amp;quot;:12}'&gt;&lt;span data-sheets-value='{&amp;quot;1&amp;quot;:2,&amp;quot;2&amp;quot;:&amp;quot;Bộ đồ chơi lắp ráp xe giúp bé phát triển kỹ năng vận động tinh thông qua các thao tác vặn, mở ốc khi chơi. Ngoài ra, bé còn rèn luyện được tư duy logic, kỹ năng khéo léo khi mày mò lắp ráp hơn 25 mảnh ghép thành 1 chiếc xe hoàn chỉnh. Bộ sản phẩm bao gồm cả vít vặn rất vừa tay cho bé ở độ tuổi preschool, nhựa chơi được trong nhà và ngoài trời/n Với nhiều chủ đề và chức năng khác nhau, hãy sưu tập đủ bộ để có thể giáo dục bé về các phương tiện có thật trong cuộc sống&amp;quot;}' data-sheets-userformat='{&amp;quot;2&amp;quot;:10685,&amp;quot;3&amp;quot;:{&amp;quot;1&amp;quot;:0,&amp;quot;3&amp;quot;:1},&amp;quot;5&amp;quot;:{&amp;quot;1&amp;quot;:[{&amp;quot;1&amp;quot;:2,&amp;quot;2&amp;quot;:0,&amp;quot;5&amp;quot;:{&amp;quot;1&amp;quot;:2,&amp;quot;2&amp;quot;:0}},{&amp;quot;1&amp;quot;:0,&amp;quot;2&amp;quot;:0,&amp;quot;3&amp;quot;:3},{&amp;quot;1&amp;quot;:1,&amp;quot;2&amp;quot;:0,&amp;quot;4&amp;quot;:1}]},&amp;quot;6&amp;quot;:{&amp;quot;1&amp;quot;:[{&amp;quot;1&amp;quot;:2,&amp;quot;2&amp;quot;:0,&amp;quot;5&amp;quot;:{&amp;quot;1&amp;quot;:2,&amp;quot;2&amp;quot;:0}},{&amp;quot;1&amp;quot;:0,&amp;quot;2&amp;quot;:0,&amp;quot;3&amp;quot;:3},{&amp;quot;1&amp;quot;:1,&amp;quot;2&amp;quot;:0,&amp;quot;4&amp;quot;:1}]},&amp;quot;7&amp;quot;:{&amp;quot;1&amp;quot;:[{&amp;quot;1&amp;quot;:2,&amp;quot;2&amp;quot;:0,&amp;quot;5&amp;quot;:{&amp;quot;1&amp;quot;:2,&amp;quot;2&amp;quot;:0}},{&amp;quot;1&amp;quot;:0,&amp;quot;2&amp;quot;:0,&amp;quot;3&amp;quot;:3},{&amp;quot;1&amp;quot;:1,&amp;quot;2&amp;quot;:0,&amp;quot;4&amp;quot;:1}]},&amp;quot;8&amp;quot;:{&amp;quot;1&amp;quot;:[{&amp;quot;1&amp;quot;:2,&amp;quot;2&amp;quot;:0,&amp;quot;5&amp;quot;:{&amp;quot;1&amp;quot;:2,&amp;quot;2&amp;quot;:0}},{&amp;quot;1&amp;quot;:0,&amp;quot;2&amp;quot;:0,&amp;quot;3&amp;quot;:3},{&amp;quot;1&amp;quot;:1,&amp;quot;2&amp;quot;:0,&amp;quot;4&amp;quot;:1}]},&amp;quot;10&amp;quot;:0,&amp;quot;11&amp;quot;:4,&amp;quot;14&amp;quot;:{&amp;quot;1&amp;quot;:3,&amp;quot;3&amp;quot;:1},&amp;quot;16&amp;quot;:12}'&gt;&lt;/span&gt;&lt;/span&gt;&lt;/p&gt;
+&lt;ul&gt;
+&lt;li&gt;Thương hiệu: VECTO&lt;/li&gt;
+&lt;li&gt;Xuất xứ thương hiệu: Việt Nam&lt;/li&gt;
+&lt;li&gt;Chất liệu: Nhựa cao cấp&lt;/li&gt;
+&lt;li&gt;Độ tuổi: 4+&lt;/li&gt;
+&lt;li&gt;Giới tính: Bé trai&lt;/li&gt;
+&lt;/ul&gt;
+&lt;p class='page-title-wrapper complex'&gt;&lt;span data-sheets-value='{&amp;quot;1&amp;quot;:2,&amp;quot;2&amp;quot;:&amp;quot;Bộ đồ chơi lắp ráp xe giúp bé phát triển kỹ năng vận động tinh thông qua các thao tác vặn, mở ốc khi chơi. Ngoài ra, bé còn rèn luyện được tư duy logic, kỹ năng khéo léo khi mày mò lắp ráp hơn 25 mảnh ghép thành 1 chiếc xe hoàn chỉnh. Bộ sản phẩm bao gồm cả vít vặn rất vừa tay cho bé ở độ tuổi preschool, nhựa chơi được trong nhà và ngoài trời/n Với nhiều chủ đề và chức năng khác nhau, hãy sưu tập đủ bộ để có thể giáo dục bé về các phương tiện có thật trong cuộc sống&amp;quot;}' data-sheets-userformat='{&amp;quot;2&amp;quot;:10685,&amp;quot;3&amp;quot;:{&amp;quot;1&amp;quot;:0,&amp;quot;3&amp;quot;:1},&amp;quot;5&amp;quot;:{&amp;quot;1&amp;quot;:[{&amp;quot;1&amp;quot;:2,&amp;quot;2&amp;quot;:0,&amp;quot;5&amp;quot;:{&amp;quot;1&amp;quot;:2,&amp;quot;2&amp;quot;:0}},{&amp;quot;1&amp;quot;:0,&amp;quot;2&amp;quot;:0,&amp;quot;3&amp;quot;:3},{&amp;quot;1&amp;quot;:1,&amp;quot;2&amp;quot;:0,&amp;quot;4&amp;quot;:1}]},&amp;quot;6&amp;quot;:{&amp;quot;1&amp;quot;:[{&amp;quot;1&amp;quot;:2,&amp;quot;2&amp;quot;:0,&amp;quot;5&amp;quot;:{&amp;quot;1&amp;quot;:2,&amp;quot;2&amp;quot;:0}},{&amp;quot;1&amp;quot;:0,&amp;quot;2&amp;quot;:0,&amp;quot;3&amp;quot;:3},{&amp;quot;1&amp;quot;:1,&amp;quot;2&amp;quot;:0,&amp;quot;4&amp;quot;:1}]},&amp;quot;7&amp;quot;:{&amp;quot;1&amp;quot;:[{&amp;quot;1&amp;quot;:2,&amp;quot;2&amp;quot;:0,&amp;quot;5&amp;quot;:{&amp;quot;1&amp;quot;:2,&amp;quot;2&amp;quot;:0}},{&amp;quot;1&amp;quot;:0,&amp;quot;2&amp;quot;:0,&amp;quot;3&amp;quot;:3},{&amp;quot;1&amp;quot;:1,&amp;quot;2&amp;quot;:0,&amp;quot;4&amp;quot;:1}]},&amp;quot;8&amp;quot;:{&amp;quot;1&amp;quot;:[{&amp;quot;1&amp;quot;:2,&amp;quot;2&amp;quot;:0,&amp;quot;5&amp;quot;:{&amp;quot;1&amp;quot;:2,&amp;quot;2&amp;quot;:0}},{&amp;quot;1&amp;quot;:0,&amp;quot;2&amp;quot;:0,&amp;quot;3&amp;quot;:3},{&amp;quot;1&amp;quot;:1,&amp;quot;2&amp;quot;:0,&amp;quot;4&amp;quot;:1}]},&amp;quot;10&amp;quot;:0,&amp;quot;11&amp;quot;:4,&amp;quot;14&amp;quot;:{&amp;quot;1&amp;quot;:3,&amp;quot;3&amp;quot;:1},&amp;quot;16&amp;quot;:12}'&gt;&lt;span data-sheets-value='{&amp;quot;1&amp;quot;:2,&amp;quot;2&amp;quot;:&amp;quot;Bộ đồ chơi lắp ráp xe giúp bé phát triển kỹ năng vận động tinh thông qua các thao tác vặn, mở ốc khi chơi. Ngoài ra, bé còn rèn luyện được tư duy logic, kỹ năng khéo léo khi mày mò lắp ráp hơn 25 mảnh ghép thành 1 chiếc xe hoàn chỉnh. Bộ sản phẩm bao gồm cả vít vặn rất vừa tay cho bé ở độ tuổi preschool, nhựa chơi được trong nhà và ngoài trời/n Với nhiều chủ đề và chức năng khác nhau, hãy sưu tập đủ bộ để có thể giáo dục bé về các phương tiện có thật trong cuộc sống&amp;quot;}' data-sheets-userformat='{&amp;quot;2&amp;quot;:10685,&amp;quot;3&amp;quot;:{&amp;quot;1&amp;quot;:0,&amp;quot;3&amp;quot;:1},&amp;quot;5&amp;quot;:{&amp;quot;1&amp;quot;:[{&amp;quot;1&amp;quot;:2,&amp;quot;2&amp;quot;:0,&amp;quot;5&amp;quot;:{&amp;quot;1&amp;quot;:2,&amp;quot;2&amp;quot;:0}},{&amp;quot;1&amp;quot;:0,&amp;quot;2&amp;quot;:0,&amp;quot;3&amp;quot;:3},{&amp;quot;1&amp;quot;:1,&amp;quot;2&amp;quot;:0,&amp;quot;4&amp;quot;:1}]},&amp;quot;6&amp;quot;:{&amp;quot;1&amp;quot;:[{&amp;quot;1&amp;quot;:2,&amp;quot;2&amp;quot;:0,&amp;quot;5&amp;quot;:{&amp;quot;1&amp;quot;:2,&amp;quot;2&amp;quot;:0}},{&amp;quot;1&amp;quot;:0,&amp;quot;2&amp;quot;:0,&amp;quot;3&amp;quot;:3},{&amp;quot;1&amp;quot;:1,&amp;quot;2&amp;quot;:0,&amp;quot;4&amp;quot;:1}]},&amp;quot;7&amp;quot;:{&amp;quot;1&amp;quot;:[{&amp;quot;1&amp;quot;:2,&amp;quot;2&amp;quot;:0,&amp;quot;5&amp;quot;:{&amp;quot;1&amp;quot;:2,&amp;quot;2&amp;quot;:0}},{&amp;quot;1&amp;quot;:0,&amp;quot;2&amp;quot;:0,&amp;quot;3&amp;quot;:3},{&amp;quot;1&amp;quot;:1,&amp;quot;2&amp;quot;:0,&amp;quot;4&amp;quot;:1}]},&amp;quot;8&amp;quot;:{&amp;quot;1&amp;quot;:[{&amp;quot;1&amp;quot;:2,&amp;quot;2&amp;quot;:0,&amp;quot;5&amp;quot;:{&amp;quot;1&amp;quot;:2,&amp;quot;2&amp;quot;:0}},{&amp;quot;1&amp;quot;:0,&amp;quot;2&amp;quot;:0,&amp;quot;3&amp;quot;:3},{&amp;quot;1&amp;quot;:1,&amp;quot;2&amp;quot;:0,&amp;quot;4&amp;quot;:1}]},&amp;quot;10&amp;quot;:0,&amp;quot;11&amp;quot;:4,&amp;quot;14&amp;quot;:{&amp;quot;1&amp;quot;:3,&amp;quot;3&amp;quot;:1},&amp;quot;16&amp;quot;:12}'&gt;&lt;/span&gt;&lt;/span&gt;&lt;/p&gt;
+&lt;/div&gt;
+&lt;div class='page-title-wrapper complex'&gt;&lt;span&gt;VECTO là thương hiệu đồ chơi dành cho bé trai. Được tạo ra để đem đến cho các bé những món đồ chơi an toàn, chất lượng, mang lại thật nhiều niềm vui đồng thời giúp bé phát triển các giác quan, kỹ năng. VECTO có rất nhiều sản phẩm đa dạng được chia thành các chủ đề: xe điều khiển từ xa, robot điều khiển từ xa, đồ chơi bay, đồ chơi lắp ráp, mô hình các phương tiện, xe lửa chạy pin….&lt;/span&gt;&lt;/div&gt;</t>
   </si>
 </sst>
 </file>
@@ -1153,10 +1159,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J33"/>
+  <dimension ref="A1:L33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K15" sqref="K15"/>
+      <selection activeCell="F33" sqref="F33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1164,7 +1170,7 @@
     <col min="6" max="6" width="17.08984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1195,8 +1201,14 @@
       <c r="J1" s="1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K1" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>10</v>
       </c>
@@ -1213,24 +1225,30 @@
         <v>13</v>
       </c>
       <c r="F2" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="G2" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="H2" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="H2" s="1" t="s">
+      <c r="I2" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="I2" s="1" t="s">
+      <c r="J2" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="J2" s="1" t="s">
+      <c r="K2">
+        <v>3</v>
+      </c>
+      <c r="L2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
         <v>18</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>19</v>
       </c>
       <c r="B3" s="1">
         <v>599000</v>
@@ -1242,27 +1260,33 @@
         <v>12</v>
       </c>
       <c r="E3" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="G3" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="F3" s="1" t="s">
+      <c r="H3" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="G3" s="1" t="s">
+      <c r="I3" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="H3" s="1" t="s">
+      <c r="J3" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="I3" s="1" t="s">
+      <c r="K3">
+        <v>3</v>
+      </c>
+      <c r="L3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
         <v>24</v>
-      </c>
-      <c r="J3" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>26</v>
       </c>
       <c r="B4" s="1">
         <v>599000</v>
@@ -1274,27 +1298,33 @@
         <v>12</v>
       </c>
       <c r="E4" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="H4" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="F4" s="1" t="s">
+      <c r="I4" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="G4" s="1" t="s">
+      <c r="J4" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="H4" s="1" t="s">
+      <c r="K4">
+        <v>3</v>
+      </c>
+      <c r="L4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
         <v>30</v>
-      </c>
-      <c r="I4" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="J4" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
-        <v>33</v>
       </c>
       <c r="B5" s="1">
         <v>599000</v>
@@ -1306,27 +1336,33 @@
         <v>12</v>
       </c>
       <c r="E5" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="I5" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="F5" s="1" t="s">
+      <c r="J5" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="G5" s="1" t="s">
+      <c r="K5">
+        <v>1</v>
+      </c>
+      <c r="L5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
         <v>36</v>
-      </c>
-      <c r="H5" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="I5" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="J5" s="1" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
-        <v>40</v>
       </c>
       <c r="B6" s="1">
         <v>349000</v>
@@ -1338,27 +1374,33 @@
         <v>12</v>
       </c>
       <c r="E6" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="I6" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="F6" s="1" t="s">
+      <c r="J6" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="G6" s="1" t="s">
+      <c r="K6">
+        <v>2</v>
+      </c>
+      <c r="L6">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
         <v>43</v>
-      </c>
-      <c r="H6" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="I6" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="J6" s="1" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
-        <v>47</v>
       </c>
       <c r="B7" s="1">
         <v>119000</v>
@@ -1370,27 +1412,33 @@
         <v>12</v>
       </c>
       <c r="E7" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="I7" s="1" t="s">
         <v>48</v>
-      </c>
-      <c r="F7" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="G7" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="H7" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="I7" s="1" t="s">
-        <v>52</v>
       </c>
       <c r="J7" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="8" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K7">
+        <v>3</v>
+      </c>
+      <c r="L7">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="B8" s="1">
         <v>119000</v>
@@ -1402,27 +1450,33 @@
         <v>12</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="F8" s="1" t="s">
         <v>11</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="J8" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="9" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K8">
+        <v>2</v>
+      </c>
+      <c r="L8">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="B9" s="1">
         <v>119000</v>
@@ -1434,27 +1488,33 @@
         <v>12</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="F9" s="1" t="s">
         <v>11</v>
       </c>
       <c r="G9" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="I9" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="J9" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="K9">
+        <v>1</v>
+      </c>
+      <c r="L9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
         <v>60</v>
-      </c>
-      <c r="H9" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="I9" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="J9" s="1" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
-        <v>64</v>
       </c>
       <c r="B10" s="1">
         <v>359000</v>
@@ -1466,27 +1526,33 @@
         <v>12</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="F10" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="I10" s="1" t="s">
         <v>65</v>
-      </c>
-      <c r="G10" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="H10" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="I10" s="1" t="s">
-        <v>69</v>
       </c>
       <c r="J10" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="11" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K10">
+        <v>3</v>
+      </c>
+      <c r="L10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="B11" s="1">
         <v>349000</v>
@@ -1498,27 +1564,33 @@
         <v>12</v>
       </c>
       <c r="E11" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="I11" s="1" t="s">
         <v>71</v>
-      </c>
-      <c r="F11" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="G11" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="H11" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="I11" s="1" t="s">
-        <v>75</v>
       </c>
       <c r="J11" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="12" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K11">
+        <v>2</v>
+      </c>
+      <c r="L11">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="B12" s="1">
         <v>359000</v>
@@ -1530,27 +1602,33 @@
         <v>12</v>
       </c>
       <c r="E12" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="H12" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="I12" s="1" t="s">
         <v>77</v>
-      </c>
-      <c r="F12" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="G12" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="H12" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="I12" s="1" t="s">
-        <v>81</v>
       </c>
       <c r="J12" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="13" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K12">
+        <v>1</v>
+      </c>
+      <c r="L12">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="B13" s="1">
         <v>349000</v>
@@ -1562,27 +1640,33 @@
         <v>12</v>
       </c>
       <c r="E13" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="H13" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="I13" s="1" t="s">
         <v>83</v>
-      </c>
-      <c r="F13" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="G13" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="H13" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="I13" s="1" t="s">
-        <v>87</v>
       </c>
       <c r="J13" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="14" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K13">
+        <v>2</v>
+      </c>
+      <c r="L13">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="B14" s="1">
         <v>349000</v>
@@ -1594,27 +1678,33 @@
         <v>12</v>
       </c>
       <c r="E14" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="H14" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="I14" s="1" t="s">
         <v>89</v>
-      </c>
-      <c r="F14" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="G14" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="H14" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="I14" s="1" t="s">
-        <v>93</v>
       </c>
       <c r="J14" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="15" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K14">
+        <v>3</v>
+      </c>
+      <c r="L14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="B15" s="1">
         <v>349000</v>
@@ -1626,27 +1716,33 @@
         <v>12</v>
       </c>
       <c r="E15" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="H15" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="I15" s="1" t="s">
         <v>95</v>
-      </c>
-      <c r="F15" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="G15" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="H15" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="I15" s="1" t="s">
-        <v>99</v>
       </c>
       <c r="J15" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="16" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K15">
+        <v>3</v>
+      </c>
+      <c r="L15">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="B16" s="1">
         <v>349000</v>
@@ -1658,27 +1754,33 @@
         <v>12</v>
       </c>
       <c r="E16" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="G16" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="H16" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="I16" s="1" t="s">
         <v>101</v>
-      </c>
-      <c r="F16" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="G16" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="H16" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="I16" s="1" t="s">
-        <v>105</v>
       </c>
       <c r="J16" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="17" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K16">
+        <v>2</v>
+      </c>
+      <c r="L16">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="B17" s="1">
         <v>119000</v>
@@ -1690,27 +1792,33 @@
         <v>12</v>
       </c>
       <c r="E17" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="G17" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="H17" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="I17" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="F17" s="1" t="s">
+      <c r="J17" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="G17" s="1" t="s">
+      <c r="K17">
+        <v>1</v>
+      </c>
+      <c r="L17">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
         <v>109</v>
-      </c>
-      <c r="H17" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="I17" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="J17" s="1" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="1" t="s">
-        <v>113</v>
       </c>
       <c r="B18" s="1">
         <v>549000</v>
@@ -1719,30 +1827,36 @@
         <v>0</v>
       </c>
       <c r="D18" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="G18" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="H18" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="I18" s="1" t="s">
         <v>114</v>
-      </c>
-      <c r="E18" s="1" t="s">
-        <v>115</v>
-      </c>
-      <c r="F18" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="G18" s="1" t="s">
-        <v>117</v>
-      </c>
-      <c r="H18" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="I18" s="1" t="s">
-        <v>119</v>
       </c>
       <c r="J18" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="19" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K18">
+        <v>2</v>
+      </c>
+      <c r="L18">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="B19" s="1">
         <v>529000</v>
@@ -1751,30 +1865,36 @@
         <v>0</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="F19" s="1" t="s">
         <v>11</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="H19" s="1" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="I19" s="1" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
       <c r="J19" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="20" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K19">
+        <v>3</v>
+      </c>
+      <c r="L19">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="B20" s="1">
         <v>159000</v>
@@ -1783,30 +1903,36 @@
         <v>0</v>
       </c>
       <c r="D20" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="G20" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="H20" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="I20" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="E20" s="1" t="s">
+      <c r="J20" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="F20" s="1" t="s">
+      <c r="K20">
+        <v>3</v>
+      </c>
+      <c r="L20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
         <v>129</v>
-      </c>
-      <c r="G20" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="H20" s="1" t="s">
-        <v>131</v>
-      </c>
-      <c r="I20" s="1" t="s">
-        <v>132</v>
-      </c>
-      <c r="J20" s="1" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="21" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="1" t="s">
-        <v>134</v>
       </c>
       <c r="B21" s="1">
         <v>259000</v>
@@ -1815,30 +1941,36 @@
         <v>0</v>
       </c>
       <c r="D21" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="G21" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="H21" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="I21" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="E21" s="1" t="s">
+      <c r="J21" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="F21" s="1" t="s">
+      <c r="K21">
+        <v>3</v>
+      </c>
+      <c r="L21">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
         <v>137</v>
-      </c>
-      <c r="G21" s="1" t="s">
-        <v>138</v>
-      </c>
-      <c r="H21" s="1" t="s">
-        <v>139</v>
-      </c>
-      <c r="I21" s="1" t="s">
-        <v>140</v>
-      </c>
-      <c r="J21" s="1" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="22" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="1" t="s">
-        <v>142</v>
       </c>
       <c r="B22" s="1">
         <v>699000</v>
@@ -1847,30 +1979,36 @@
         <v>0</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>145</v>
+        <v>204</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>146</v>
+        <v>140</v>
       </c>
       <c r="H22" s="1" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
       <c r="I22" s="1" t="s">
-        <v>148</v>
+        <v>142</v>
       </c>
       <c r="J22" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="23" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K22">
+        <v>2</v>
+      </c>
+      <c r="L22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>149</v>
+        <v>143</v>
       </c>
       <c r="B23" s="1">
         <v>699000</v>
@@ -1879,30 +2017,36 @@
         <v>0</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>150</v>
+        <v>144</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>151</v>
+        <v>205</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>152</v>
+        <v>145</v>
       </c>
       <c r="H23" s="1" t="s">
-        <v>153</v>
+        <v>146</v>
       </c>
       <c r="I23" s="1" t="s">
-        <v>154</v>
+        <v>147</v>
       </c>
       <c r="J23" s="1" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="24" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>148</v>
+      </c>
+      <c r="K23">
+        <v>1</v>
+      </c>
+      <c r="L23">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>156</v>
+        <v>149</v>
       </c>
       <c r="B24" s="1">
         <v>639000</v>
@@ -1911,30 +2055,36 @@
         <v>0</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>157</v>
+        <v>150</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>158</v>
+        <v>151</v>
       </c>
       <c r="G24" s="1" t="s">
-        <v>159</v>
+        <v>152</v>
       </c>
       <c r="H24" s="1" t="s">
-        <v>160</v>
+        <v>153</v>
       </c>
       <c r="I24" s="1" t="s">
-        <v>161</v>
+        <v>154</v>
       </c>
       <c r="J24" s="1" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="25" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>155</v>
+      </c>
+      <c r="K24">
+        <v>3</v>
+      </c>
+      <c r="L24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>163</v>
+        <v>156</v>
       </c>
       <c r="B25" s="1">
         <v>569000</v>
@@ -1943,30 +2093,36 @@
         <v>0</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>164</v>
+        <v>157</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>165</v>
+        <v>158</v>
       </c>
       <c r="G25" s="1" t="s">
-        <v>166</v>
+        <v>159</v>
       </c>
       <c r="H25" s="1" t="s">
-        <v>167</v>
+        <v>160</v>
       </c>
       <c r="I25" s="1" t="s">
-        <v>168</v>
+        <v>161</v>
       </c>
       <c r="J25" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="26" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K25">
+        <v>3</v>
+      </c>
+      <c r="L25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>169</v>
+        <v>162</v>
       </c>
       <c r="B26" s="1">
         <v>599000</v>
@@ -1975,30 +2131,36 @@
         <v>0</v>
       </c>
       <c r="D26" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="F26" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="G26" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="H26" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="I26" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="J26" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="K26">
+        <v>2</v>
+      </c>
+      <c r="L26">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="1" t="s">
         <v>170</v>
-      </c>
-      <c r="E26" s="1" t="s">
-        <v>171</v>
-      </c>
-      <c r="F26" s="1" t="s">
-        <v>172</v>
-      </c>
-      <c r="G26" s="1" t="s">
-        <v>173</v>
-      </c>
-      <c r="H26" s="1" t="s">
-        <v>174</v>
-      </c>
-      <c r="I26" s="1" t="s">
-        <v>175</v>
-      </c>
-      <c r="J26" s="1" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="27" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="1" t="s">
-        <v>177</v>
       </c>
       <c r="B27" s="1">
         <v>999000</v>
@@ -2007,19 +2169,19 @@
         <v>0</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>178</v>
+        <v>171</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>179</v>
+        <v>172</v>
       </c>
       <c r="G27" s="1" t="s">
-        <v>180</v>
+        <v>173</v>
       </c>
       <c r="H27" s="1" t="s">
-        <v>181</v>
+        <v>174</v>
       </c>
       <c r="I27" s="1" t="s">
         <v>11</v>
@@ -2027,10 +2189,16 @@
       <c r="J27" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="28" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K27">
+        <v>1</v>
+      </c>
+      <c r="L27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
-        <v>182</v>
+        <v>175</v>
       </c>
       <c r="B28" s="1">
         <v>1199000</v>
@@ -2039,19 +2207,19 @@
         <v>0</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>183</v>
+        <v>176</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>184</v>
+        <v>206</v>
       </c>
       <c r="G28" s="1" t="s">
-        <v>185</v>
+        <v>177</v>
       </c>
       <c r="H28" s="1" t="s">
-        <v>186</v>
+        <v>178</v>
       </c>
       <c r="I28" s="1" t="s">
         <v>11</v>
@@ -2059,10 +2227,16 @@
       <c r="J28" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="29" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K28">
+        <v>3</v>
+      </c>
+      <c r="L28">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
-        <v>187</v>
+        <v>179</v>
       </c>
       <c r="B29" s="1">
         <v>699000</v>
@@ -2071,19 +2245,19 @@
         <v>0</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>188</v>
+        <v>180</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>189</v>
+        <v>181</v>
       </c>
       <c r="G29" s="1" t="s">
-        <v>190</v>
+        <v>182</v>
       </c>
       <c r="H29" s="1" t="s">
-        <v>191</v>
+        <v>183</v>
       </c>
       <c r="I29" s="1" t="s">
         <v>11</v>
@@ -2091,10 +2265,16 @@
       <c r="J29" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="30" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K29">
+        <v>3</v>
+      </c>
+      <c r="L29">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
-        <v>192</v>
+        <v>184</v>
       </c>
       <c r="B30" s="1">
         <v>699000</v>
@@ -2103,30 +2283,36 @@
         <v>0</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>193</v>
+        <v>185</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>194</v>
+        <v>186</v>
       </c>
       <c r="G30" s="1" t="s">
-        <v>195</v>
+        <v>187</v>
       </c>
       <c r="H30" s="1" t="s">
-        <v>196</v>
+        <v>188</v>
       </c>
       <c r="I30" s="1" t="s">
-        <v>197</v>
+        <v>189</v>
       </c>
       <c r="J30" s="1" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="31" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>190</v>
+      </c>
+      <c r="K30">
+        <v>1</v>
+      </c>
+      <c r="L30">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="B31" s="1">
         <v>159000</v>
@@ -2135,30 +2321,36 @@
         <v>0</v>
       </c>
       <c r="D31" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="E31" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="F31" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="G31" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="H31" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="I31" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="E31" s="1" t="s">
+      <c r="J31" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="F31" s="1" t="s">
-        <v>129</v>
-      </c>
-      <c r="G31" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="H31" s="1" t="s">
-        <v>131</v>
-      </c>
-      <c r="I31" s="1" t="s">
-        <v>132</v>
-      </c>
-      <c r="J31" s="1" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="32" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K31">
+        <v>1</v>
+      </c>
+      <c r="L31">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
-        <v>199</v>
+        <v>191</v>
       </c>
       <c r="B32" s="1">
         <v>839000</v>
@@ -2167,30 +2359,36 @@
         <v>0</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="E32" s="1">
         <v>6058417</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>200</v>
+        <v>192</v>
       </c>
       <c r="G32" s="1" t="s">
-        <v>201</v>
+        <v>193</v>
       </c>
       <c r="H32" s="1" t="s">
-        <v>202</v>
+        <v>194</v>
       </c>
       <c r="I32" s="1" t="s">
-        <v>203</v>
+        <v>195</v>
       </c>
       <c r="J32" s="1" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="33" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>196</v>
+      </c>
+      <c r="K32">
+        <v>1</v>
+      </c>
+      <c r="L32">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
-        <v>199</v>
+        <v>191</v>
       </c>
       <c r="B33" s="1">
         <v>839000</v>
@@ -2199,31 +2397,37 @@
         <v>0</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="E33" s="1">
         <v>6058417</v>
       </c>
       <c r="F33" s="1" t="s">
-        <v>200</v>
+        <v>192</v>
       </c>
       <c r="G33" s="1" t="s">
-        <v>201</v>
+        <v>193</v>
       </c>
       <c r="H33" s="1" t="s">
-        <v>202</v>
+        <v>194</v>
       </c>
       <c r="I33" s="1" t="s">
-        <v>203</v>
+        <v>195</v>
       </c>
       <c r="J33" s="1" t="s">
-        <v>204</v>
+        <v>196</v>
+      </c>
+      <c r="K33">
+        <v>1</v>
+      </c>
+      <c r="L33">
+        <v>3</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError sqref="A1:J1 A2 A3 A4 A5 A6 D6:J6 A7 D7:J7 A8 A9 D9:J9 A10 A11 D11:J11 A12 A13 A14 D14:J14 A15 A16 A17 A18 A19 A20 A21 A22 A23 A24 A25 A26 A27 A28 A29 D2:E2 D3:J3 D4:J4 D5:J5 D8:J8 D10:J10 D12:J12 D13:J13 D15:J15 D16:J16 D17:J17 D18:J18 D19:J19 D20:J20 D21:J21 D22:J22 D23:J23 D24:J24 D25:J25 D26:J26 D27:J27 D28:J28 D29:J29 G2:J2" numberStoredAsText="1"/>
+    <ignoredError sqref="A1:J1 A2 A3 A4 A5 A6 D6:J6 A7 D7:J7 A8 A9 D9:J9 A10 A11 D11:J11 A12 A13 A14 D14:J14 A15 A16 A17 A18 A19 A20 A21 A22 A23 A24 A25 A26 A27 A28 A29 D2:E2 D3:E3 D4:E4 D5:E5 D8:J8 D10:J10 D12:J12 D13:J13 D15:J15 D16:J16 D17:J17 D18:E18 D19:J19 D20:J20 D21:J21 D22:E22 D23:E23 D24:J24 D25:J25 D26:J26 D27:J27 D28:E28 D29:J29 G2:J2 G22:J22 G3:J3 G4:J4 G5:J5 G18:J18 G23:J23 G28:J28" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>